<commit_message>
cambiato ore del consuntivo
</commit_message>
<xml_diff>
--- a/SWE/Documentazione/Piano_di_Progetto/file sorgenti/Piano orario.xlsx
+++ b/SWE/Documentazione/Piano_di_Progetto/file sorgenti/Piano orario.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="15120" windowHeight="8010" activeTab="6"/>
@@ -15,7 +15,7 @@
     <sheet name="Resoconto finale" sheetId="6" r:id="rId6"/>
     <sheet name="tabelle forma carina" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="351">
   <si>
     <t>Identificativo</t>
   </si>
@@ -1098,29 +1098,86 @@
     <t>an</t>
   </si>
   <si>
-    <t>15(+1)</t>
-  </si>
-  <si>
-    <t>16(+1)</t>
-  </si>
-  <si>
-    <t>11(-1)</t>
-  </si>
-  <si>
-    <t>20(21)</t>
-  </si>
-  <si>
-    <t>19(20)</t>
-  </si>
-  <si>
-    <t>21(20)</t>
+    <t>8(-1)</t>
+  </si>
+  <si>
+    <t>10(-1)</t>
+  </si>
+  <si>
+    <t>10(-3)</t>
+  </si>
+  <si>
+    <t>24(-7)</t>
+  </si>
+  <si>
+    <t>49(+12)</t>
+  </si>
+  <si>
+    <t>143(+1)</t>
+  </si>
+  <si>
+    <t>Totale Consuntivo</t>
+  </si>
+  <si>
+    <t>Totale Preventivo</t>
+  </si>
+  <si>
+    <t>Differenza</t>
+  </si>
+  <si>
+    <t>1(-1)</t>
+  </si>
+  <si>
+    <t>8(-3)</t>
+  </si>
+  <si>
+    <t>12(-4)</t>
+  </si>
+  <si>
+    <t>3(+1)</t>
+  </si>
+  <si>
+    <t>18(+3)</t>
+  </si>
+  <si>
+    <t>0(+4)</t>
+  </si>
+  <si>
+    <t>20(+4)</t>
+  </si>
+  <si>
+    <t>28(+2)</t>
+  </si>
+  <si>
+    <t>30(-1)</t>
+  </si>
+  <si>
+    <t>16(+2)</t>
+  </si>
+  <si>
+    <t>10(-2)</t>
+  </si>
+  <si>
+    <t>4(-2)</t>
+  </si>
+  <si>
+    <t>31(+2)</t>
+  </si>
+  <si>
+    <t>34(-1)</t>
+  </si>
+  <si>
+    <t>33(+2)</t>
+  </si>
+  <si>
+    <t>35(-1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1194,6 +1251,21 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1416,7 +1488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1635,12 +1707,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1653,12 +1719,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1690,11 +1761,31 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2001,11 +2092,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="111710592"/>
-        <c:axId val="111712128"/>
+        <c:axId val="88395136"/>
+        <c:axId val="88413312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111710592"/>
+        <c:axId val="88395136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2014,7 +2105,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111712128"/>
+        <c:crossAx val="88413312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2022,7 +2113,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111712128"/>
+        <c:axId val="88413312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2033,7 +2124,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111710592"/>
+        <c:crossAx val="88395136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2511,11 +2602,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="112386048"/>
-        <c:axId val="112387584"/>
+        <c:axId val="88087552"/>
+        <c:axId val="88101632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="112386048"/>
+        <c:axId val="88087552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2524,7 +2615,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112387584"/>
+        <c:crossAx val="88101632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2532,7 +2623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112387584"/>
+        <c:axId val="88101632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2543,7 +2634,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112386048"/>
+        <c:crossAx val="88087552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3269,11 +3360,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="113077632"/>
-        <c:axId val="113079424"/>
+        <c:axId val="92969600"/>
+        <c:axId val="92971392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113077632"/>
+        <c:axId val="92969600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3282,7 +3373,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113079424"/>
+        <c:crossAx val="92971392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3290,7 +3381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113079424"/>
+        <c:axId val="92971392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3301,7 +3392,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113077632"/>
+        <c:crossAx val="92969600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3671,22 +3762,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>118</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>243</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>293</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3806,19 +3897,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>920</c:v>
+                  <c:v>860</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1530</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2950</c:v>
+                  <c:v>2775</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3645</c:v>
+                  <c:v>3825</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6446</c:v>
+                  <c:v>6468</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2430</c:v>
@@ -3872,19 +3963,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>720</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>675</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>3030</c:v>
+                  <c:v>3210</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6446</c:v>
+                  <c:v>6468</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2430</c:v>
@@ -4008,19 +4099,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>202</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>293</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>162</c:v>
@@ -4144,19 +4235,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>720</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>675</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>3030</c:v>
+                  <c:v>3210</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6446</c:v>
+                  <c:v>6468</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2430</c:v>
@@ -4442,7 +4533,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>8</c:v>
@@ -4511,7 +4602,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>4</c:v>
@@ -4586,13 +4677,13 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5</c:v>
@@ -4733,16 +4824,16 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>33</c:v>
@@ -4802,22 +4893,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>55</c:v>
@@ -4836,11 +4927,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="113119232"/>
-        <c:axId val="113120768"/>
+        <c:axId val="93277184"/>
+        <c:axId val="93291264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113119232"/>
+        <c:axId val="93277184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4849,7 +4940,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113120768"/>
+        <c:crossAx val="93291264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4857,7 +4948,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113120768"/>
+        <c:axId val="93291264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4868,7 +4959,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113119232"/>
+        <c:crossAx val="93277184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4994,7 +5085,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -5063,7 +5154,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
@@ -5138,13 +5229,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -5285,16 +5376,16 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>21</c:v>
@@ -5354,22 +5445,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>55</c:v>
@@ -5388,11 +5479,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="113157632"/>
-        <c:axId val="113159168"/>
+        <c:axId val="93319936"/>
+        <c:axId val="93321472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113157632"/>
+        <c:axId val="93319936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5401,7 +5492,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113159168"/>
+        <c:crossAx val="93321472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5409,7 +5500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113159168"/>
+        <c:axId val="93321472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5420,7 +5511,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113157632"/>
+        <c:crossAx val="93319936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5875,11 +5966,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="111896448"/>
-        <c:axId val="111897984"/>
+        <c:axId val="91855488"/>
+        <c:axId val="91857280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111896448"/>
+        <c:axId val="91855488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5888,7 +5979,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111897984"/>
+        <c:crossAx val="91857280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5896,7 +5987,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111897984"/>
+        <c:axId val="91857280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5907,7 +5998,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111896448"/>
+        <c:crossAx val="91855488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6580,11 +6671,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="112296320"/>
-        <c:axId val="112297856"/>
+        <c:axId val="92263936"/>
+        <c:axId val="92265472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="112296320"/>
+        <c:axId val="92263936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6593,7 +6684,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112297856"/>
+        <c:crossAx val="92265472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6601,7 +6692,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112297856"/>
+        <c:axId val="92265472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6612,7 +6703,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112296320"/>
+        <c:crossAx val="92263936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7913,12 +8004,12 @@
       <c r="N1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="97" t="s">
+      <c r="O1" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C2" s="61"/>
@@ -7927,12 +8018,12 @@
       <c r="N2" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="96" t="s">
+      <c r="O2" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="97"/>
+      <c r="R2" s="97"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -7947,11 +8038,11 @@
       <c r="N3" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="96" t="s">
+      <c r="O3" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="96"/>
-      <c r="Q3" s="96"/>
+      <c r="P3" s="97"/>
+      <c r="Q3" s="97"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -7973,12 +8064,12 @@
       <c r="N4" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="96" t="s">
+      <c r="O4" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="96"/>
-      <c r="Q4" s="96"/>
-      <c r="R4" s="96"/>
+      <c r="P4" s="97"/>
+      <c r="Q4" s="97"/>
+      <c r="R4" s="97"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -8000,12 +8091,12 @@
       <c r="N5" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="96" t="s">
+      <c r="O5" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="96"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
+      <c r="P5" s="97"/>
+      <c r="Q5" s="97"/>
+      <c r="R5" s="97"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -8027,12 +8118,12 @@
       <c r="N6" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="96" t="s">
+      <c r="O6" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="96"/>
-      <c r="Q6" s="96"/>
-      <c r="R6" s="96"/>
+      <c r="P6" s="97"/>
+      <c r="Q6" s="97"/>
+      <c r="R6" s="97"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -8047,12 +8138,12 @@
       <c r="N7" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="96" t="s">
+      <c r="O7" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="96"/>
-      <c r="Q7" s="96"/>
-      <c r="R7" s="96"/>
+      <c r="P7" s="97"/>
+      <c r="Q7" s="97"/>
+      <c r="R7" s="97"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -9457,7 +9548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
@@ -12716,8 +12807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR36"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12739,56 +12830,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="101" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="J1" s="98" t="s">
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="J1" s="99" t="s">
         <v>289</v>
       </c>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="S1" s="98" t="s">
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
+      <c r="S1" s="99" t="s">
         <v>290</v>
       </c>
-      <c r="T1" s="98"/>
-      <c r="U1" s="98"/>
-      <c r="V1" s="98"/>
-      <c r="W1" s="98"/>
-      <c r="X1" s="98"/>
-      <c r="Y1" s="98"/>
-      <c r="Z1" s="98"/>
-      <c r="AB1" s="98" t="s">
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="X1" s="99"/>
+      <c r="Y1" s="99"/>
+      <c r="Z1" s="99"/>
+      <c r="AB1" s="99" t="s">
         <v>219</v>
       </c>
-      <c r="AC1" s="98"/>
-      <c r="AD1" s="98"/>
-      <c r="AE1" s="98"/>
-      <c r="AF1" s="98"/>
-      <c r="AG1" s="98"/>
-      <c r="AH1" s="98"/>
-      <c r="AI1" s="98"/>
-      <c r="AK1" s="98" t="s">
+      <c r="AC1" s="99"/>
+      <c r="AD1" s="99"/>
+      <c r="AE1" s="99"/>
+      <c r="AF1" s="99"/>
+      <c r="AG1" s="99"/>
+      <c r="AH1" s="99"/>
+      <c r="AI1" s="99"/>
+      <c r="AK1" s="99" t="s">
         <v>291</v>
       </c>
-      <c r="AL1" s="98"/>
-      <c r="AM1" s="98"/>
-      <c r="AN1" s="98"/>
-      <c r="AO1" s="98"/>
-      <c r="AP1" s="98"/>
-      <c r="AQ1" s="98"/>
-      <c r="AR1" s="98"/>
+      <c r="AL1" s="99"/>
+      <c r="AM1" s="99"/>
+      <c r="AN1" s="99"/>
+      <c r="AO1" s="99"/>
+      <c r="AP1" s="99"/>
+      <c r="AQ1" s="99"/>
+      <c r="AR1" s="99"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
@@ -12899,14 +12990,14 @@
         <v>80</v>
       </c>
       <c r="T4" s="61">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U4" s="61">
         <v>20</v>
       </c>
       <c r="V4" s="61">
-        <f>T4*U4</f>
-        <v>200</v>
+        <f>U4*T4</f>
+        <v>140</v>
       </c>
       <c r="W4" s="51"/>
       <c r="X4" s="51"/>
@@ -12978,14 +13069,14 @@
         <v>90</v>
       </c>
       <c r="T5" s="61">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="U5" s="61">
         <v>30</v>
       </c>
-      <c r="V5" s="61">
-        <f>T5*U5</f>
-        <v>300</v>
+      <c r="V5" s="93">
+        <f t="shared" ref="V5:V9" si="0">U5*T5</f>
+        <v>270</v>
       </c>
       <c r="W5" s="51"/>
       <c r="X5" s="51"/>
@@ -13031,7 +13122,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="61">
-        <f t="shared" ref="D6:D7" si="0">B6*C6</f>
+        <f t="shared" ref="D6:D7" si="1">B6*C6</f>
         <v>1575</v>
       </c>
       <c r="E6" s="51"/>
@@ -13047,7 +13138,7 @@
         <v>25</v>
       </c>
       <c r="M6" s="61">
-        <f t="shared" ref="M6:M7" si="1">K6*L6</f>
+        <f t="shared" ref="M6:M7" si="2">K6*L6</f>
         <v>700</v>
       </c>
       <c r="N6" s="51"/>
@@ -13057,15 +13148,14 @@
         <v>188</v>
       </c>
       <c r="T6" s="61">
-        <f>8+6+6+4</f>
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="U6" s="61">
         <v>25</v>
       </c>
-      <c r="V6" s="61">
-        <f>T6*U6</f>
-        <v>600</v>
+      <c r="V6" s="93">
+        <f t="shared" si="0"/>
+        <v>425</v>
       </c>
       <c r="W6" s="51"/>
       <c r="X6" s="51"/>
@@ -13080,7 +13170,7 @@
         <v>25</v>
       </c>
       <c r="AE6" s="61">
-        <f t="shared" ref="AE6:AE7" si="2">AC6*AD6</f>
+        <f t="shared" ref="AE6:AE7" si="3">AC6*AD6</f>
         <v>75</v>
       </c>
       <c r="AF6" s="51"/>
@@ -13094,7 +13184,7 @@
         <v>25</v>
       </c>
       <c r="AN6" s="61">
-        <f t="shared" ref="AN6:AN7" si="3">AL6*AM6</f>
+        <f t="shared" ref="AN6:AN7" si="4">AL6*AM6</f>
         <v>0</v>
       </c>
       <c r="AO6" s="51"/>
@@ -13110,7 +13200,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>495</v>
       </c>
       <c r="E7" s="51"/>
@@ -13126,7 +13216,7 @@
         <v>15</v>
       </c>
       <c r="M7" s="61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="N7" s="51"/>
@@ -13136,14 +13226,14 @@
         <v>126</v>
       </c>
       <c r="T7" s="61">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="U7" s="61">
         <v>15</v>
       </c>
-      <c r="V7" s="61">
-        <f>T7*U7</f>
-        <v>735</v>
+      <c r="V7" s="93">
+        <f t="shared" si="0"/>
+        <v>915</v>
       </c>
       <c r="W7" s="51"/>
       <c r="X7" s="51"/>
@@ -13157,7 +13247,7 @@
         <v>15</v>
       </c>
       <c r="AE7" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1215</v>
       </c>
       <c r="AF7" s="51"/>
@@ -13171,7 +13261,7 @@
         <v>15</v>
       </c>
       <c r="AN7" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1080</v>
       </c>
       <c r="AO7" s="51"/>
@@ -13213,14 +13303,14 @@
         <v>187</v>
       </c>
       <c r="T8" s="61">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U8" s="61">
         <v>22</v>
       </c>
-      <c r="V8" s="61">
-        <f>T8*U8</f>
-        <v>3146</v>
+      <c r="V8" s="93">
+        <f t="shared" si="0"/>
+        <v>3168</v>
       </c>
       <c r="W8" s="51"/>
       <c r="X8" s="51"/>
@@ -13295,7 +13385,8 @@
       <c r="U9" s="61">
         <v>15</v>
       </c>
-      <c r="V9" s="61">
+      <c r="V9" s="93">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W9" s="51"/>
@@ -13363,11 +13454,12 @@
       <c r="S10" s="61"/>
       <c r="T10" s="61">
         <f>SUM(T4:T9)</f>
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="U10" s="61"/>
       <c r="V10" s="61">
-        <v>5199</v>
+        <f>SUM(V4:V9)</f>
+        <v>4918</v>
       </c>
       <c r="W10" s="51"/>
       <c r="X10" s="51" t="s">
@@ -13564,11 +13656,11 @@
         <v>3</v>
       </c>
       <c r="Y14" s="61">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Z14" s="61">
         <f>SUM(T14:Y14)</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="AB14" s="12" t="s">
         <v>281</v>
@@ -13639,7 +13731,7 @@
       <c r="O15" s="61"/>
       <c r="P15" s="51"/>
       <c r="Q15" s="51">
-        <f t="shared" ref="Q15:Q20" si="4">SUM(K15:O15)</f>
+        <f t="shared" ref="Q15:Q20" si="5">SUM(K15:O15)</f>
         <v>5</v>
       </c>
       <c r="S15" s="14" t="s">
@@ -13656,7 +13748,7 @@
         <v>29</v>
       </c>
       <c r="Z15" s="61">
-        <f t="shared" ref="Z15:Z19" si="5">SUM(T15:Y15)</f>
+        <f t="shared" ref="Z15:Z19" si="6">SUM(T15:Y15)</f>
         <v>35</v>
       </c>
       <c r="AB15" s="14" t="s">
@@ -13730,7 +13822,7 @@
       <c r="O16" s="61"/>
       <c r="P16" s="51"/>
       <c r="Q16" s="51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="S16" s="10" t="s">
@@ -13741,10 +13833,10 @@
       <c r="V16" s="61"/>
       <c r="W16" s="61"/>
       <c r="X16" s="61">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y16" s="61">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Z16" s="61">
         <f>SUM(T16:Y16)</f>
@@ -13823,7 +13915,7 @@
       <c r="O17" s="61"/>
       <c r="P17" s="51"/>
       <c r="Q17" s="51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="S17" s="22" t="s">
@@ -13831,19 +13923,19 @@
       </c>
       <c r="T17" s="61"/>
       <c r="U17" s="61">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="V17" s="61">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W17" s="61"/>
       <c r="X17" s="61">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="Y17" s="61"/>
       <c r="Z17" s="61">
-        <f t="shared" si="5"/>
-        <v>34</v>
+        <f t="shared" si="6"/>
+        <v>33</v>
       </c>
       <c r="AB17" s="22" t="s">
         <v>284</v>
@@ -13861,7 +13953,7 @@
         <v>27</v>
       </c>
       <c r="AI17" s="61">
-        <f t="shared" ref="AI17:AI19" si="6">SUM(AC17:AH17)</f>
+        <f t="shared" ref="AI17:AI19" si="7">SUM(AC17:AH17)</f>
         <v>52</v>
       </c>
       <c r="AK17" s="22" t="s">
@@ -13882,7 +13974,7 @@
         <v>15</v>
       </c>
       <c r="AR17" s="61">
-        <f t="shared" ref="AR17:AR19" si="7">SUM(AL17:AQ17)</f>
+        <f t="shared" ref="AR17:AR19" si="8">SUM(AL17:AQ17)</f>
         <v>19</v>
       </c>
     </row>
@@ -13920,7 +14012,7 @@
       </c>
       <c r="P18" s="51"/>
       <c r="Q18" s="51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="S18" s="16" t="s">
@@ -13933,18 +14025,18 @@
         <v>2</v>
       </c>
       <c r="V18" s="61">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="W18" s="61"/>
       <c r="X18" s="61">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y18" s="61">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="Z18" s="61">
         <f>SUM(T18:Y18)</f>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AB18" s="16" t="s">
         <v>285</v>
@@ -14002,7 +14094,7 @@
       </c>
       <c r="G19" s="51"/>
       <c r="H19" s="51">
-        <f t="shared" ref="H19" si="8">B19+C19+D19+F19</f>
+        <f t="shared" ref="H19" si="9">B19+C19+D19+F19</f>
         <v>18</v>
       </c>
       <c r="J19" s="9" t="s">
@@ -14017,29 +14109,29 @@
       <c r="O19" s="61"/>
       <c r="P19" s="51"/>
       <c r="Q19" s="51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="S19" s="9" t="s">
         <v>286</v>
       </c>
       <c r="T19" s="61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U19" s="61"/>
       <c r="V19" s="61">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W19" s="61"/>
       <c r="X19" s="61">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="Y19" s="61">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Z19" s="61">
-        <f t="shared" si="5"/>
-        <v>35</v>
+        <f t="shared" si="6"/>
+        <v>34</v>
       </c>
       <c r="AB19" s="9" t="s">
         <v>286</v>
@@ -14059,7 +14151,7 @@
         <v>27</v>
       </c>
       <c r="AI19" s="61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>49</v>
       </c>
       <c r="AK19" s="9" t="s">
@@ -14078,7 +14170,7 @@
         <v>8</v>
       </c>
       <c r="AR19" s="61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
     </row>
@@ -14118,7 +14210,7 @@
       </c>
       <c r="P20" s="51"/>
       <c r="Q20" s="51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="S20" s="20" t="s">
@@ -14184,18 +14276,18 @@
         <v>24</v>
       </c>
       <c r="C21" s="52">
-        <f t="shared" ref="C21:D21" si="9">SUM(C14:C20)</f>
+        <f t="shared" ref="C21:D21" si="10">SUM(C14:C20)</f>
         <v>19</v>
       </c>
       <c r="D21" s="52">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>63</v>
       </c>
       <c r="E21" s="52">
         <v>0</v>
       </c>
       <c r="F21" s="62">
-        <f t="shared" ref="F21" si="10">SUM(F14:F20)</f>
+        <f t="shared" ref="F21" si="11">SUM(F14:F20)</f>
         <v>33</v>
       </c>
       <c r="G21" s="52">
@@ -14211,66 +14303,66 @@
         <v>3</v>
       </c>
       <c r="L21" s="52">
-        <f t="shared" ref="L21:Q21" si="11">SUM(L14:L20)</f>
+        <f t="shared" ref="L21:Q21" si="12">SUM(L14:L20)</f>
         <v>2</v>
       </c>
       <c r="M21" s="52">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>28</v>
       </c>
       <c r="N21" s="52">
         <v>0</v>
       </c>
       <c r="O21" s="62">
-        <f t="shared" ref="O21" si="12">SUM(O14:O20)</f>
+        <f t="shared" ref="O21" si="13">SUM(O14:O20)</f>
         <v>8</v>
       </c>
       <c r="P21" s="52">
         <v>0</v>
       </c>
       <c r="Q21" s="52">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>41</v>
       </c>
       <c r="S21" s="6"/>
       <c r="T21" s="62">
-        <f t="shared" ref="T21:Y21" si="13">SUM(T14:T20)</f>
-        <v>10</v>
+        <f t="shared" ref="T21:Y21" si="14">SUM(T14:T20)</f>
+        <v>9</v>
       </c>
       <c r="U21" s="62">
-        <f t="shared" si="13"/>
-        <v>10</v>
+        <f t="shared" si="14"/>
+        <v>7</v>
       </c>
       <c r="V21" s="62">
-        <f t="shared" si="13"/>
-        <v>24</v>
+        <f t="shared" si="14"/>
+        <v>17</v>
       </c>
       <c r="W21" s="62">
         <v>0</v>
       </c>
       <c r="X21" s="62">
-        <f t="shared" si="13"/>
-        <v>49</v>
+        <f t="shared" si="14"/>
+        <v>61</v>
       </c>
       <c r="Y21" s="62">
-        <f t="shared" si="13"/>
-        <v>143</v>
+        <f t="shared" si="14"/>
+        <v>144</v>
       </c>
       <c r="Z21" s="62">
         <f>SUM(Z14:Z20)</f>
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AB21" s="6"/>
       <c r="AC21" s="62">
-        <f t="shared" ref="AC21:AH21" si="14">SUM(AC14:AC20)</f>
+        <f t="shared" ref="AC21:AH21" si="15">SUM(AC14:AC20)</f>
         <v>8</v>
       </c>
       <c r="AD21" s="62">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7</v>
       </c>
       <c r="AE21" s="62">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="AF21" s="62">
@@ -14278,11 +14370,11 @@
         <v>132</v>
       </c>
       <c r="AG21" s="62">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>81</v>
       </c>
       <c r="AH21" s="62">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>114</v>
       </c>
       <c r="AI21" s="62">
@@ -14291,15 +14383,15 @@
       </c>
       <c r="AK21" s="6"/>
       <c r="AL21" s="62">
-        <f t="shared" ref="AL21:AQ21" si="15">SUM(AL14:AL20)</f>
+        <f t="shared" ref="AL21:AQ21" si="16">SUM(AL14:AL20)</f>
         <v>6</v>
       </c>
       <c r="AM21" s="62">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AN21" s="62">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AO21" s="62">
@@ -14307,11 +14399,11 @@
         <v>30</v>
       </c>
       <c r="AP21" s="62">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>72</v>
       </c>
       <c r="AQ21" s="62">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>36</v>
       </c>
       <c r="AR21" s="62">
@@ -14320,26 +14412,26 @@
       </c>
     </row>
     <row r="27" spans="1:44" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H27" s="99" t="s">
+      <c r="H27" s="100" t="s">
         <v>307</v>
       </c>
-      <c r="I27" s="99"/>
-      <c r="J27" s="99"/>
-      <c r="K27" s="99"/>
-      <c r="L27" s="99"/>
-      <c r="M27" s="99"/>
-      <c r="N27" s="99"/>
-      <c r="O27" s="99"/>
-      <c r="W27" s="99" t="s">
+      <c r="I27" s="100"/>
+      <c r="J27" s="100"/>
+      <c r="K27" s="100"/>
+      <c r="L27" s="100"/>
+      <c r="M27" s="100"/>
+      <c r="N27" s="100"/>
+      <c r="O27" s="100"/>
+      <c r="W27" s="100" t="s">
         <v>308</v>
       </c>
-      <c r="X27" s="98"/>
-      <c r="Y27" s="98"/>
-      <c r="Z27" s="98"/>
-      <c r="AA27" s="98"/>
-      <c r="AB27" s="98"/>
-      <c r="AC27" s="98"/>
-      <c r="AD27" s="98"/>
+      <c r="X27" s="99"/>
+      <c r="Y27" s="99"/>
+      <c r="Z27" s="99"/>
+      <c r="AA27" s="99"/>
+      <c r="AB27" s="99"/>
+      <c r="AC27" s="99"/>
+      <c r="AD27" s="99"/>
     </row>
     <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -14428,19 +14520,19 @@
       </c>
       <c r="C29">
         <f>T4+AC4+AL4</f>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D29">
         <f>B29+C29</f>
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E29">
         <f>C29*C4</f>
-        <v>500</v>
+        <v>440</v>
       </c>
       <c r="F29">
         <f>D29*C4</f>
-        <v>920</v>
+        <v>860</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>281</v>
@@ -14450,28 +14542,28 @@
         <v>13</v>
       </c>
       <c r="J29" s="51">
-        <f t="shared" ref="J29:N35" si="16">C14+L14+U14+AD14+AM14</f>
+        <f t="shared" ref="J29:N35" si="17">C14+L14+U14+AD14+AM14</f>
         <v>10</v>
       </c>
       <c r="K29" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="L29" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>28</v>
       </c>
       <c r="M29" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>29</v>
       </c>
       <c r="N29" s="51">
-        <f t="shared" si="16"/>
-        <v>46</v>
+        <f t="shared" si="17"/>
+        <v>48</v>
       </c>
       <c r="O29" s="51">
         <f>SUM(I29:N29)</f>
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="P29" s="51"/>
       <c r="Q29" s="51"/>
@@ -14484,43 +14576,43 @@
       </c>
       <c r="T29" s="58">
         <f>Z14+AI14+AR14</f>
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="U29" s="58">
         <f>S29+T29</f>
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="V29" s="58"/>
       <c r="W29" s="12" t="s">
         <v>281</v>
       </c>
       <c r="X29" s="61">
-        <f t="shared" ref="X29:AC35" si="17">T14+AC14+AL14</f>
+        <f t="shared" ref="X29:AC35" si="18">T14+AC14+AL14</f>
         <v>5</v>
       </c>
       <c r="Y29" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Z29" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AA29" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>28</v>
       </c>
       <c r="AB29" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>26</v>
       </c>
       <c r="AC29" s="61">
-        <f t="shared" si="17"/>
-        <v>46</v>
+        <f t="shared" si="18"/>
+        <v>48</v>
       </c>
       <c r="AD29" s="61">
         <f>SUM(X29:AC29)</f>
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:44" x14ac:dyDescent="0.25">
@@ -14528,42 +14620,42 @@
         <v>90</v>
       </c>
       <c r="B30">
-        <f t="shared" ref="B30:B34" si="18">B5+K5</f>
+        <f t="shared" ref="B30:B34" si="19">B5+K5</f>
         <v>27</v>
       </c>
       <c r="C30">
         <f>T5+AC5+AL5</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D30">
         <f>B30+C30</f>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E30">
-        <f t="shared" ref="E30:E34" si="19">C30*C5</f>
-        <v>720</v>
+        <f t="shared" ref="E30:E34" si="20">C30*C5</f>
+        <v>690</v>
       </c>
       <c r="F30">
-        <f t="shared" ref="F30:F33" si="20">D30*C5</f>
-        <v>1530</v>
+        <f t="shared" ref="F30:F33" si="21">D30*C5</f>
+        <v>1500</v>
       </c>
       <c r="H30" s="14" t="s">
         <v>282</v>
       </c>
       <c r="I30" s="51">
-        <f t="shared" ref="I30:I35" si="21">B15+K15+T15+AC15+AL15</f>
+        <f t="shared" ref="I30:I35" si="22">B15+K15+T15+AC15+AL15</f>
         <v>6</v>
       </c>
       <c r="J30" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3</v>
       </c>
       <c r="K30" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="L30" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>28</v>
       </c>
       <c r="M30" s="51">
@@ -14571,11 +14663,11 @@
         <v>25</v>
       </c>
       <c r="N30" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>47</v>
       </c>
       <c r="O30" s="51">
-        <f t="shared" ref="O30:O35" si="22">SUM(I30:N30)</f>
+        <f t="shared" ref="O30:O35" si="23">SUM(I30:N30)</f>
         <v>129</v>
       </c>
       <c r="P30" s="51"/>
@@ -14588,11 +14680,11 @@
         <v>25</v>
       </c>
       <c r="T30" s="58">
-        <f t="shared" ref="T30:T35" si="23">Z15+AI15+AR15</f>
+        <f t="shared" ref="T30:T35" si="24">Z15+AI15+AR15</f>
         <v>104</v>
       </c>
       <c r="U30" s="58">
-        <f t="shared" ref="U30:U36" si="24">S30+T30</f>
+        <f t="shared" ref="U30:U36" si="25">S30+T30</f>
         <v>129</v>
       </c>
       <c r="V30" s="58"/>
@@ -14600,31 +14692,31 @@
         <v>282</v>
       </c>
       <c r="X30" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="Y30" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="Z30" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AA30" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>28</v>
       </c>
       <c r="AB30" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>20</v>
       </c>
       <c r="AC30" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>47</v>
       </c>
       <c r="AD30" s="61">
-        <f t="shared" ref="AD30:AD35" si="25">SUM(X30:AC30)</f>
+        <f t="shared" ref="AD30:AD35" si="26">SUM(X30:AC30)</f>
         <v>104</v>
       </c>
     </row>
@@ -14633,54 +14725,54 @@
         <v>188</v>
       </c>
       <c r="B31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>91</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:C34" si="26">T6+AC6+AL6</f>
-        <v>27</v>
+        <f t="shared" ref="C31:C34" si="27">T6+AC6+AL6</f>
+        <v>20</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D34" si="27">B31+C31</f>
-        <v>118</v>
+        <f t="shared" ref="D31:D34" si="28">B31+C31</f>
+        <v>111</v>
       </c>
       <c r="E31">
-        <f t="shared" si="19"/>
-        <v>675</v>
+        <f t="shared" si="20"/>
+        <v>500</v>
       </c>
       <c r="F31">
-        <f t="shared" si="20"/>
-        <v>2950</v>
+        <f t="shared" si="21"/>
+        <v>2775</v>
       </c>
       <c r="H31" s="10" t="s">
         <v>283</v>
       </c>
       <c r="I31" s="51">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="J31" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
       <c r="K31" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>19</v>
       </c>
       <c r="L31" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>38</v>
       </c>
       <c r="M31" s="51">
-        <f t="shared" si="16"/>
-        <v>23</v>
+        <f t="shared" si="17"/>
+        <v>24</v>
       </c>
       <c r="N31" s="51">
-        <f t="shared" si="16"/>
-        <v>30</v>
+        <f t="shared" si="17"/>
+        <v>29</v>
       </c>
       <c r="O31" s="51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>131</v>
       </c>
       <c r="P31" s="51"/>
@@ -14689,15 +14781,15 @@
         <v>283</v>
       </c>
       <c r="S31" s="58">
-        <f t="shared" ref="S31:S35" si="28">H16+Q16</f>
+        <f t="shared" ref="S31:S35" si="29">H16+Q16</f>
         <v>26</v>
       </c>
       <c r="T31" s="58">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>105</v>
       </c>
       <c r="U31" s="58">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>131</v>
       </c>
       <c r="V31" s="58"/>
@@ -14705,31 +14797,31 @@
         <v>283</v>
       </c>
       <c r="X31" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="Y31" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="Z31" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AA31" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>38</v>
       </c>
       <c r="AB31" s="61">
-        <f t="shared" si="17"/>
-        <v>23</v>
+        <f t="shared" si="18"/>
+        <v>24</v>
       </c>
       <c r="AC31" s="61">
-        <f t="shared" si="17"/>
-        <v>30</v>
+        <f t="shared" si="18"/>
+        <v>29</v>
       </c>
       <c r="AD31" s="61">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>105</v>
       </c>
     </row>
@@ -14738,55 +14830,55 @@
         <v>126</v>
       </c>
       <c r="B32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>41</v>
       </c>
       <c r="C32">
-        <f t="shared" si="26"/>
-        <v>202</v>
+        <f t="shared" si="27"/>
+        <v>214</v>
       </c>
       <c r="D32">
-        <f t="shared" si="27"/>
-        <v>243</v>
+        <f t="shared" si="28"/>
+        <v>255</v>
       </c>
       <c r="E32">
-        <f t="shared" si="19"/>
-        <v>3030</v>
+        <f t="shared" si="20"/>
+        <v>3210</v>
       </c>
       <c r="F32">
-        <f t="shared" si="20"/>
-        <v>3645</v>
+        <f t="shared" si="21"/>
+        <v>3825</v>
       </c>
       <c r="H32" s="22" t="s">
         <v>284</v>
       </c>
       <c r="I32" s="51">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4</v>
       </c>
       <c r="J32" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="K32" s="51">
+        <f t="shared" si="17"/>
+        <v>26</v>
+      </c>
+      <c r="L32" s="51">
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
-      <c r="K32" s="51">
-        <f t="shared" si="16"/>
-        <v>27</v>
-      </c>
-      <c r="L32" s="51">
-        <f t="shared" si="16"/>
-        <v>10</v>
-      </c>
       <c r="M32" s="51">
-        <f t="shared" si="16"/>
-        <v>37</v>
+        <f t="shared" si="17"/>
+        <v>40</v>
       </c>
       <c r="N32" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>42</v>
       </c>
       <c r="O32" s="51">
-        <f t="shared" si="22"/>
-        <v>130</v>
+        <f t="shared" si="23"/>
+        <v>129</v>
       </c>
       <c r="P32" s="51"/>
       <c r="Q32" s="51"/>
@@ -14794,48 +14886,48 @@
         <v>284</v>
       </c>
       <c r="S32" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>25</v>
       </c>
       <c r="T32" s="58">
-        <f t="shared" si="23"/>
-        <v>105</v>
+        <f t="shared" si="24"/>
+        <v>104</v>
       </c>
       <c r="U32" s="58">
-        <f t="shared" si="24"/>
-        <v>130</v>
+        <f t="shared" si="25"/>
+        <v>129</v>
       </c>
       <c r="V32" s="58"/>
       <c r="W32" s="22" t="s">
         <v>284</v>
       </c>
       <c r="X32" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="Y32" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
+        <v>7</v>
+      </c>
+      <c r="Z32" s="61">
+        <f t="shared" si="18"/>
+        <v>7</v>
+      </c>
+      <c r="AA32" s="61">
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
-      <c r="Z32" s="61">
-        <f t="shared" si="17"/>
-        <v>8</v>
-      </c>
-      <c r="AA32" s="61">
-        <f t="shared" si="17"/>
-        <v>10</v>
-      </c>
       <c r="AB32" s="61">
-        <f t="shared" si="17"/>
-        <v>34</v>
+        <f t="shared" si="18"/>
+        <v>37</v>
       </c>
       <c r="AC32" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>42</v>
       </c>
       <c r="AD32" s="61">
-        <f t="shared" si="25"/>
-        <v>105</v>
+        <f t="shared" si="26"/>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
@@ -14843,24 +14935,24 @@
         <v>187</v>
       </c>
       <c r="B33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="C33">
         <f>T8+AC8+AL8</f>
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D33">
         <f>B33+C33</f>
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E33">
-        <f t="shared" si="19"/>
-        <v>6446</v>
+        <f t="shared" si="20"/>
+        <v>6468</v>
       </c>
       <c r="F33">
-        <f t="shared" si="20"/>
-        <v>6446</v>
+        <f t="shared" si="21"/>
+        <v>6468</v>
       </c>
       <c r="H33" s="16" t="s">
         <v>285</v>
@@ -14870,28 +14962,28 @@
         <v>3</v>
       </c>
       <c r="J33" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="K33" s="51">
-        <f t="shared" si="16"/>
-        <v>33</v>
+        <f t="shared" si="17"/>
+        <v>29</v>
       </c>
       <c r="L33" s="51">
         <f>E18+N18+W18+AF18+AO18</f>
         <v>20</v>
       </c>
       <c r="M33" s="51">
-        <f t="shared" si="16"/>
-        <v>45</v>
+        <f t="shared" si="17"/>
+        <v>49</v>
       </c>
       <c r="N33" s="51">
-        <f t="shared" si="16"/>
-        <v>28</v>
+        <f t="shared" si="17"/>
+        <v>30</v>
       </c>
       <c r="O33" s="51">
-        <f t="shared" si="22"/>
-        <v>133</v>
+        <f t="shared" si="23"/>
+        <v>135</v>
       </c>
       <c r="P33" s="51"/>
       <c r="Q33" s="51"/>
@@ -14899,48 +14991,48 @@
         <v>285</v>
       </c>
       <c r="S33" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>28</v>
       </c>
       <c r="T33" s="58">
-        <f t="shared" si="23"/>
-        <v>105</v>
+        <f t="shared" si="24"/>
+        <v>107</v>
       </c>
       <c r="U33" s="58">
-        <f t="shared" si="24"/>
-        <v>133</v>
+        <f t="shared" si="25"/>
+        <v>135</v>
       </c>
       <c r="V33" s="58"/>
       <c r="W33" s="16" t="s">
         <v>285</v>
       </c>
       <c r="X33" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="Y33" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="Z33" s="61">
-        <f t="shared" si="17"/>
-        <v>15</v>
+        <f t="shared" si="18"/>
+        <v>11</v>
       </c>
       <c r="AA33" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>20</v>
       </c>
       <c r="AB33" s="61">
-        <f t="shared" si="17"/>
-        <v>37</v>
+        <f t="shared" si="18"/>
+        <v>41</v>
       </c>
       <c r="AC33" s="61">
-        <f t="shared" si="17"/>
-        <v>28</v>
+        <f t="shared" si="18"/>
+        <v>30</v>
       </c>
       <c r="AD33" s="61">
-        <f t="shared" si="25"/>
-        <v>105</v>
+        <f t="shared" si="26"/>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
@@ -14948,19 +15040,19 @@
         <v>224</v>
       </c>
       <c r="B34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="C34">
-        <f t="shared" si="26"/>
-        <v>162</v>
-      </c>
-      <c r="D34">
         <f t="shared" si="27"/>
         <v>162</v>
       </c>
+      <c r="D34">
+        <f t="shared" si="28"/>
+        <v>162</v>
+      </c>
       <c r="E34">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2430</v>
       </c>
       <c r="F34">
@@ -14971,32 +15063,32 @@
         <v>286</v>
       </c>
       <c r="I34" s="51">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <f t="shared" si="22"/>
+        <v>8</v>
       </c>
       <c r="J34" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="K34" s="51">
-        <f t="shared" si="16"/>
-        <v>9</v>
+        <f t="shared" si="17"/>
+        <v>7</v>
       </c>
       <c r="L34" s="51">
         <f>E19+N19+W19+AF19+AO19</f>
         <v>10</v>
       </c>
       <c r="M34" s="51">
-        <f t="shared" si="16"/>
-        <v>51</v>
+        <f t="shared" si="17"/>
+        <v>55</v>
       </c>
       <c r="N34" s="51">
-        <f t="shared" si="16"/>
-        <v>45</v>
+        <f t="shared" si="17"/>
+        <v>43</v>
       </c>
       <c r="O34" s="51">
-        <f t="shared" si="22"/>
-        <v>128</v>
+        <f t="shared" si="23"/>
+        <v>127</v>
       </c>
       <c r="P34" s="51"/>
       <c r="Q34" s="51"/>
@@ -15004,48 +15096,48 @@
         <v>286</v>
       </c>
       <c r="S34" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>23</v>
       </c>
       <c r="T34" s="58">
-        <f t="shared" si="23"/>
-        <v>105</v>
+        <f t="shared" si="24"/>
+        <v>104</v>
       </c>
       <c r="U34" s="58">
-        <f t="shared" si="24"/>
-        <v>128</v>
+        <f t="shared" si="25"/>
+        <v>127</v>
       </c>
       <c r="V34" s="58"/>
       <c r="W34" s="9" t="s">
         <v>286</v>
       </c>
       <c r="X34" s="61">
-        <f t="shared" si="17"/>
-        <v>1</v>
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="Y34" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="Z34" s="61">
-        <f t="shared" si="17"/>
-        <v>4</v>
+        <f t="shared" si="18"/>
+        <v>2</v>
       </c>
       <c r="AA34" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
       <c r="AB34" s="61">
-        <f t="shared" si="17"/>
-        <v>41</v>
+        <f t="shared" si="18"/>
+        <v>45</v>
       </c>
       <c r="AC34" s="61">
-        <f t="shared" si="17"/>
-        <v>45</v>
+        <f t="shared" si="18"/>
+        <v>43</v>
       </c>
       <c r="AD34" s="61">
-        <f t="shared" si="25"/>
-        <v>105</v>
+        <f t="shared" si="26"/>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.25">
@@ -15053,24 +15145,24 @@
         <v>294</v>
       </c>
       <c r="B35">
-        <f t="shared" ref="B35" si="29">SUM(B29:B34)</f>
+        <f t="shared" ref="B35" si="30">SUM(B29:B34)</f>
         <v>180</v>
       </c>
       <c r="C35">
         <f>SUM(C29:C34)</f>
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="D35">
         <f>SUM(D29:D34)</f>
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="E35">
         <f>SUM(E29:E34)</f>
-        <v>13801</v>
+        <v>13738</v>
       </c>
       <c r="F35">
         <f>SUM(F29:F34)</f>
-        <v>17921</v>
+        <v>17858</v>
       </c>
       <c r="G35" t="s">
         <v>304</v>
@@ -15079,31 +15171,31 @@
         <v>287</v>
       </c>
       <c r="I35" s="51">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="J35" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="K35" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="L35" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>28</v>
       </c>
       <c r="M35" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>33</v>
       </c>
       <c r="N35" s="51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>55</v>
       </c>
       <c r="O35" s="51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>131</v>
       </c>
       <c r="P35" s="51"/>
@@ -15112,15 +15204,15 @@
         <v>287</v>
       </c>
       <c r="S35" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>27</v>
       </c>
       <c r="T35" s="58">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>104</v>
       </c>
       <c r="U35" s="58">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>131</v>
       </c>
       <c r="V35" s="58"/>
@@ -15128,31 +15220,31 @@
         <v>287</v>
       </c>
       <c r="X35" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Y35" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Z35" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AA35" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>28</v>
       </c>
       <c r="AB35" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>21</v>
       </c>
       <c r="AC35" s="61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>55</v>
       </c>
       <c r="AD35" s="61">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>104</v>
       </c>
     </row>
@@ -15160,31 +15252,31 @@
       <c r="H36" s="6"/>
       <c r="I36" s="52">
         <f>SUM(I29:I35)</f>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J36" s="52">
-        <f t="shared" ref="J36" si="30">SUM(J29:J35)</f>
-        <v>46</v>
+        <f t="shared" ref="J36" si="31">SUM(J29:J35)</f>
+        <v>43</v>
       </c>
       <c r="K36" s="52">
-        <f t="shared" ref="K36" si="31">SUM(K29:K35)</f>
-        <v>118</v>
+        <f t="shared" ref="K36" si="32">SUM(K29:K35)</f>
+        <v>111</v>
       </c>
       <c r="L36" s="52">
         <f>SUM(L29:L35)</f>
         <v>162</v>
       </c>
       <c r="M36" s="52">
-        <f t="shared" ref="M36" si="32">SUM(M29:M35)</f>
-        <v>243</v>
+        <f t="shared" ref="M36" si="33">SUM(M29:M35)</f>
+        <v>255</v>
       </c>
       <c r="N36" s="52">
-        <f t="shared" ref="N36" si="33">SUM(N29:N35)</f>
-        <v>293</v>
+        <f t="shared" ref="N36" si="34">SUM(N29:N35)</f>
+        <v>294</v>
       </c>
       <c r="O36" s="52">
         <f>SUM(O29:O35)</f>
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="P36" s="52"/>
       <c r="Q36" s="52"/>
@@ -15194,42 +15286,42 @@
         <v>180</v>
       </c>
       <c r="T36" s="59">
-        <f t="shared" ref="T36" si="34">SUM(T29:T35)</f>
-        <v>733</v>
+        <f t="shared" ref="T36" si="35">SUM(T29:T35)</f>
+        <v>735</v>
       </c>
       <c r="U36" s="58">
-        <f t="shared" si="24"/>
-        <v>913</v>
+        <f t="shared" si="25"/>
+        <v>915</v>
       </c>
       <c r="V36" s="59"/>
       <c r="W36" s="6"/>
       <c r="X36" s="62">
         <f>SUM(X29:X35)</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Y36" s="62">
-        <f t="shared" ref="Y36:Z36" si="35">SUM(Y29:Y35)</f>
-        <v>25</v>
+        <f t="shared" ref="Y36:Z36" si="36">SUM(Y29:Y35)</f>
+        <v>22</v>
       </c>
       <c r="Z36" s="62">
-        <f t="shared" si="35"/>
-        <v>27</v>
+        <f t="shared" si="36"/>
+        <v>20</v>
       </c>
       <c r="AA36" s="62">
         <f>SUM(AA29:AA35)</f>
         <v>162</v>
       </c>
       <c r="AB36" s="62">
-        <f t="shared" ref="AB36:AC36" si="36">SUM(AB29:AB35)</f>
-        <v>202</v>
+        <f t="shared" ref="AB36:AC36" si="37">SUM(AB29:AB35)</f>
+        <v>214</v>
       </c>
       <c r="AC36" s="62">
-        <f t="shared" si="36"/>
-        <v>293</v>
+        <f t="shared" si="37"/>
+        <v>294</v>
       </c>
       <c r="AD36" s="62">
         <f>SUM(AD29:AD35)</f>
-        <v>733</v>
+        <v>735</v>
       </c>
     </row>
   </sheetData>
@@ -15252,8 +15344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15387,46 +15479,46 @@
       <c r="D9" s="65">
         <v>3</v>
       </c>
-      <c r="G9" s="105" t="s">
+      <c r="G9" s="106" t="s">
         <v>318</v>
       </c>
-      <c r="H9" s="101" t="s">
+      <c r="H9" s="102" t="s">
         <v>319</v>
       </c>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="102"/>
-      <c r="N9" s="103" t="s">
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
+      <c r="K9" s="103"/>
+      <c r="L9" s="103"/>
+      <c r="M9" s="103"/>
+      <c r="N9" s="104" t="s">
         <v>322</v>
       </c>
       <c r="P9" s="80" t="s">
         <v>186</v>
       </c>
-      <c r="Q9" s="93" t="s">
+      <c r="Q9" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="R9" s="91"/>
-      <c r="S9" s="92" t="s">
+      <c r="R9" s="89"/>
+      <c r="S9" s="90" t="s">
         <v>323</v>
       </c>
       <c r="U9" s="80" t="s">
         <v>186</v>
       </c>
-      <c r="V9" s="90" t="s">
+      <c r="V9" s="88" t="s">
         <v>292</v>
       </c>
-      <c r="W9" s="93" t="s">
+      <c r="W9" s="91" t="s">
         <v>293</v>
       </c>
-      <c r="X9" s="91" t="s">
+      <c r="X9" s="89" t="s">
         <v>294</v>
       </c>
-      <c r="Y9" s="93" t="s">
+      <c r="Y9" s="91" t="s">
         <v>324</v>
       </c>
-      <c r="Z9" s="92" t="s">
+      <c r="Z9" s="90" t="s">
         <v>95</v>
       </c>
     </row>
@@ -15443,7 +15535,7 @@
       <c r="D10" s="65">
         <v>3</v>
       </c>
-      <c r="G10" s="106"/>
+      <c r="G10" s="107"/>
       <c r="H10" s="68" t="s">
         <v>314</v>
       </c>
@@ -15462,18 +15554,19 @@
       <c r="M10" s="70" t="s">
         <v>321</v>
       </c>
-      <c r="N10" s="104"/>
+      <c r="N10" s="105"/>
       <c r="P10" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="Q10" s="85">
-        <v>8</v>
+      <c r="Q10" s="85" t="s">
+        <v>328</v>
       </c>
       <c r="R10" s="85">
         <v>20</v>
       </c>
       <c r="S10" s="73">
-        <v>160</v>
+        <f>7*20</f>
+        <v>140</v>
       </c>
       <c r="U10" s="82" t="s">
         <v>80</v>
@@ -15511,31 +15604,32 @@
         <v>281</v>
       </c>
       <c r="H11" s="65">
-        <v>8</v>
-      </c>
-      <c r="I11" s="72">
-        <v>10</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I11" s="72"/>
       <c r="J11" s="78"/>
-      <c r="K11" s="107"/>
+      <c r="K11" s="95"/>
       <c r="L11" s="72">
-        <v>2</v>
-      </c>
-      <c r="M11" s="72"/>
-      <c r="N11" s="79">
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="M11" s="72" t="s">
+        <v>342</v>
+      </c>
+      <c r="N11" s="79" t="s">
+        <v>347</v>
       </c>
       <c r="P11" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="Q11" s="73">
-        <v>6</v>
+      <c r="Q11" s="73" t="s">
+        <v>327</v>
       </c>
       <c r="R11" s="72">
         <v>30</v>
       </c>
       <c r="S11" s="86">
-        <v>180</v>
+        <f>9*30</f>
+        <v>270</v>
       </c>
       <c r="U11" s="74" t="s">
         <v>90</v>
@@ -15568,30 +15662,31 @@
       <c r="G12" s="74" t="s">
         <v>282</v>
       </c>
-      <c r="H12" s="65"/>
+      <c r="H12" s="65">
+        <v>6</v>
+      </c>
       <c r="I12" s="72"/>
-      <c r="J12" s="78" t="s">
-        <v>326</v>
-      </c>
-      <c r="K12" s="107"/>
-      <c r="L12" s="72">
-        <v>5</v>
-      </c>
-      <c r="M12" s="72"/>
-      <c r="N12" s="73" t="s">
-        <v>329</v>
+      <c r="J12" s="78"/>
+      <c r="K12" s="95"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72">
+        <v>29</v>
+      </c>
+      <c r="N12" s="73">
+        <v>35</v>
       </c>
       <c r="P12" s="72" t="s">
         <v>188</v>
       </c>
-      <c r="Q12" s="73">
-        <v>0</v>
+      <c r="Q12" s="73" t="s">
+        <v>329</v>
       </c>
       <c r="R12" s="72">
         <v>25</v>
       </c>
       <c r="S12" s="86">
-        <v>0</v>
+        <f>17*25</f>
+        <v>425</v>
       </c>
       <c r="U12" s="74" t="s">
         <v>188</v>
@@ -15629,29 +15724,30 @@
         <v>283</v>
       </c>
       <c r="H13" s="65"/>
-      <c r="I13" s="72">
-        <v>7</v>
-      </c>
-      <c r="J13" s="78">
-        <v>14</v>
-      </c>
-      <c r="K13" s="107"/>
-      <c r="L13" s="72"/>
-      <c r="M13" s="72"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="95"/>
+      <c r="L13" s="72" t="s">
+        <v>338</v>
+      </c>
+      <c r="M13" s="72" t="s">
+        <v>343</v>
+      </c>
       <c r="N13" s="73">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="P13" s="72" t="s">
         <v>126</v>
       </c>
-      <c r="Q13" s="73">
-        <v>72</v>
+      <c r="Q13" s="73" t="s">
+        <v>330</v>
       </c>
       <c r="R13" s="72">
         <v>15</v>
       </c>
       <c r="S13" s="86">
-        <v>1080</v>
+        <f>61*15</f>
+        <v>915</v>
       </c>
       <c r="U13" s="74" t="s">
         <v>126</v>
@@ -15689,29 +15785,32 @@
         <v>284</v>
       </c>
       <c r="H14" s="78"/>
-      <c r="I14" s="72"/>
+      <c r="I14" s="72" t="s">
+        <v>336</v>
+      </c>
       <c r="J14" s="78" t="s">
-        <v>327</v>
-      </c>
-      <c r="K14" s="107"/>
-      <c r="L14" s="72">
-        <v>3</v>
+        <v>326</v>
+      </c>
+      <c r="K14" s="95"/>
+      <c r="L14" s="72" t="s">
+        <v>339</v>
       </c>
       <c r="M14" s="72"/>
       <c r="N14" s="73" t="s">
-        <v>330</v>
+        <v>348</v>
       </c>
       <c r="P14" s="72" t="s">
         <v>187</v>
       </c>
-      <c r="Q14" s="73">
-        <v>36</v>
+      <c r="Q14" s="73" t="s">
+        <v>331</v>
       </c>
       <c r="R14" s="72">
         <v>22</v>
       </c>
       <c r="S14" s="86">
-        <v>792</v>
+        <f>144*22</f>
+        <v>3168</v>
       </c>
       <c r="U14" s="74" t="s">
         <v>187</v>
@@ -15748,30 +15847,36 @@
       <c r="G15" s="74" t="s">
         <v>285</v>
       </c>
-      <c r="H15" s="65"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="78">
-        <v>18</v>
-      </c>
-      <c r="K15" s="107"/>
-      <c r="L15" s="72">
+      <c r="H15" s="65">
+        <v>3</v>
+      </c>
+      <c r="I15" s="72">
         <v>2</v>
       </c>
-      <c r="M15" s="72"/>
-      <c r="N15" s="73">
-        <v>20</v>
+      <c r="J15" s="78" t="s">
+        <v>337</v>
+      </c>
+      <c r="K15" s="95"/>
+      <c r="L15" s="72" t="s">
+        <v>340</v>
+      </c>
+      <c r="M15" s="72" t="s">
+        <v>344</v>
+      </c>
+      <c r="N15" s="73" t="s">
+        <v>349</v>
       </c>
       <c r="P15" s="72" t="s">
         <v>224</v>
       </c>
       <c r="Q15" s="73">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="R15" s="72">
         <v>15</v>
       </c>
       <c r="S15" s="86">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="U15" s="74" t="s">
         <v>224</v>
@@ -15792,7 +15897,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -15808,39 +15913,44 @@
       <c r="G16" s="74" t="s">
         <v>286</v>
       </c>
-      <c r="H16" s="65">
-        <v>8</v>
+      <c r="H16" s="65" t="s">
+        <v>335</v>
       </c>
       <c r="I16" s="72"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="107"/>
-      <c r="L16" s="72">
-        <v>10</v>
-      </c>
-      <c r="M16" s="72"/>
-      <c r="N16" s="73">
-        <v>18</v>
-      </c>
-      <c r="P16" s="94" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q16" s="89">
-        <v>152</v>
-      </c>
-      <c r="R16" s="87"/>
-      <c r="S16" s="88">
-        <v>2662</v>
+      <c r="J16" s="78" t="s">
+        <v>346</v>
+      </c>
+      <c r="K16" s="95"/>
+      <c r="L16" s="72" t="s">
+        <v>341</v>
+      </c>
+      <c r="M16" s="72" t="s">
+        <v>345</v>
+      </c>
+      <c r="N16" s="73" t="s">
+        <v>350</v>
+      </c>
+      <c r="P16" s="114" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q16" s="110">
+        <v>238</v>
+      </c>
+      <c r="R16" s="109"/>
+      <c r="S16" s="110">
+        <f>SUM(S10:S15)</f>
+        <v>4918</v>
       </c>
       <c r="U16" s="83" t="s">
         <v>294</v>
       </c>
-      <c r="V16" s="95">
+      <c r="V16" s="92">
         <v>180</v>
       </c>
       <c r="W16" s="87">
         <v>733</v>
       </c>
-      <c r="X16" s="95">
+      <c r="X16" s="92">
         <v>913</v>
       </c>
       <c r="Y16" s="87">
@@ -15850,7 +15960,7 @@
         <v>17921</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -15866,23 +15976,31 @@
       <c r="G17" s="75" t="s">
         <v>287</v>
       </c>
-      <c r="H17" s="67">
-        <v>8</v>
-      </c>
-      <c r="I17" s="76">
-        <v>2</v>
-      </c>
+      <c r="H17" s="67"/>
+      <c r="I17" s="76"/>
       <c r="J17" s="77"/>
-      <c r="K17" s="108"/>
-      <c r="L17" s="76" t="s">
-        <v>328</v>
-      </c>
-      <c r="M17" s="76"/>
-      <c r="N17" s="77" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K17" s="96"/>
+      <c r="L17" s="76">
+        <v>5</v>
+      </c>
+      <c r="M17" s="76">
+        <v>30</v>
+      </c>
+      <c r="N17" s="77">
+        <v>35</v>
+      </c>
+      <c r="P17" s="72" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q17" s="111">
+        <v>236</v>
+      </c>
+      <c r="R17" s="108"/>
+      <c r="S17" s="111">
+        <v>4981</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -15891,8 +16009,20 @@
       </c>
       <c r="C18" s="65"/>
       <c r="D18" s="65"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N18" s="115"/>
+      <c r="P18" s="76" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q18" s="112">
+        <v>-2</v>
+      </c>
+      <c r="R18" s="108"/>
+      <c r="S18" s="113">
+        <f>S16-S17</f>
+        <v>-63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -15906,7 +16036,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -15920,7 +16050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -15933,8 +16063,13 @@
       <c r="D21" s="65">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q21" s="94"/>
+      <c r="R21" s="94"/>
+      <c r="S21" s="94"/>
+      <c r="T21" s="94"/>
+      <c r="U21" s="94"/>
+    </row>
+    <row r="22" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -15947,8 +16082,13 @@
       <c r="D22" s="65">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q22" s="93"/>
+      <c r="R22" s="93"/>
+      <c r="S22" s="93"/>
+      <c r="T22" s="93"/>
+      <c r="U22" s="93"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -15961,8 +16101,13 @@
       <c r="D23" s="65">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q23" s="93"/>
+      <c r="R23" s="93"/>
+      <c r="S23" s="93"/>
+      <c r="T23" s="93"/>
+      <c r="U23" s="93"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -15975,8 +16120,13 @@
       <c r="D24" s="65">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q24" s="93"/>
+      <c r="R24" s="93"/>
+      <c r="S24" s="93"/>
+      <c r="T24" s="93"/>
+      <c r="U24" s="93"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -15989,8 +16139,13 @@
       <c r="D25" s="65">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q25" s="93"/>
+      <c r="R25" s="93"/>
+      <c r="S25" s="93"/>
+      <c r="T25" s="93"/>
+      <c r="U25" s="93"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -16003,8 +16158,13 @@
       <c r="D26" s="65">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q26" s="93"/>
+      <c r="R26" s="93"/>
+      <c r="S26" s="93"/>
+      <c r="T26" s="93"/>
+      <c r="U26" s="93"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>64</v>
       </c>
@@ -16013,8 +16173,13 @@
       </c>
       <c r="C27" s="65"/>
       <c r="D27" s="65"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q27" s="93"/>
+      <c r="R27" s="93"/>
+      <c r="S27" s="93"/>
+      <c r="T27" s="93"/>
+      <c r="U27" s="93"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -16027,8 +16192,13 @@
       <c r="D28" s="65">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="Q28" s="93"/>
+      <c r="R28" s="93"/>
+      <c r="S28" s="93"/>
+      <c r="T28" s="93"/>
+      <c r="U28" s="93"/>
+    </row>
+    <row r="29" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -16042,7 +16212,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -16056,7 +16226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -16070,7 +16240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
aggiunto su pdp consuntivo e preventivo a finire
</commit_message>
<xml_diff>
--- a/SWE/Documentazione/Piano_di_Progetto/file sorgenti/Piano orario.xlsx
+++ b/SWE/Documentazione/Piano_di_Progetto/file sorgenti/Piano orario.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="15120" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="15120" windowHeight="8010" tabRatio="754" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Analisi Requisiti" sheetId="1" r:id="rId1"/>
     <sheet name="Analisi dettaglio" sheetId="2" r:id="rId2"/>
     <sheet name="Progettazione" sheetId="3" r:id="rId3"/>
     <sheet name="Codifica" sheetId="4" r:id="rId4"/>
-    <sheet name="Qualifica" sheetId="5" r:id="rId5"/>
-    <sheet name="Resoconto finale" sheetId="6" r:id="rId6"/>
-    <sheet name="tabelle forma carina" sheetId="7" r:id="rId7"/>
+    <sheet name="tabelle forma carina" sheetId="7" r:id="rId5"/>
+    <sheet name="Qualifica" sheetId="5" r:id="rId6"/>
+    <sheet name="Resoconto finale" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="372">
   <si>
     <t>Identificativo</t>
   </si>
@@ -1174,6 +1174,66 @@
   </si>
   <si>
     <t>prob consuntivo:</t>
+  </si>
+  <si>
+    <t>7(-3)</t>
+  </si>
+  <si>
+    <t>8(-4)</t>
+  </si>
+  <si>
+    <t>3(-1)</t>
+  </si>
+  <si>
+    <t>81(+25)</t>
+  </si>
+  <si>
+    <t>114(-7)</t>
+  </si>
+  <si>
+    <t>132(-2)</t>
+  </si>
+  <si>
+    <t>4(+2)</t>
+  </si>
+  <si>
+    <t>8(+1)</t>
+  </si>
+  <si>
+    <t>13(+5)</t>
+  </si>
+  <si>
+    <t>15(+3)</t>
+  </si>
+  <si>
+    <t>23(+4)</t>
+  </si>
+  <si>
+    <t>18(+5)</t>
+  </si>
+  <si>
+    <t>0(+5)</t>
+  </si>
+  <si>
+    <t>18(-2)</t>
+  </si>
+  <si>
+    <t>27(-2)</t>
+  </si>
+  <si>
+    <t>12(-1)</t>
+  </si>
+  <si>
+    <t>49(+1)</t>
+  </si>
+  <si>
+    <t>52(-1)</t>
+  </si>
+  <si>
+    <t>48(+2)</t>
+  </si>
+  <si>
+    <t>46(+5)</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1764,6 +1824,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1791,6 +1857,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2101,11 +2173,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="68035328"/>
-        <c:axId val="68036864"/>
+        <c:axId val="47977216"/>
+        <c:axId val="47978752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68035328"/>
+        <c:axId val="47977216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2114,7 +2186,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68036864"/>
+        <c:crossAx val="47978752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2122,7 +2194,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68036864"/>
+        <c:axId val="47978752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2133,7 +2205,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68035328"/>
+        <c:crossAx val="47977216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2612,11 +2684,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="71012736"/>
-        <c:axId val="71014272"/>
+        <c:axId val="47806720"/>
+        <c:axId val="47816704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71012736"/>
+        <c:axId val="47806720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2625,7 +2697,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71014272"/>
+        <c:crossAx val="47816704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2633,7 +2705,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71014272"/>
+        <c:axId val="47816704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2644,7 +2716,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71012736"/>
+        <c:crossAx val="47806720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3375,11 +3447,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="71360512"/>
-        <c:axId val="71362048"/>
+        <c:axId val="83152896"/>
+        <c:axId val="83154432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71360512"/>
+        <c:axId val="83152896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3388,7 +3460,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71362048"/>
+        <c:crossAx val="83154432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3396,7 +3468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71362048"/>
+        <c:axId val="83154432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3407,14 +3479,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71360512"/>
+        <c:crossAx val="83152896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4947,11 +5018,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="71680384"/>
-        <c:axId val="71681920"/>
+        <c:axId val="86622592"/>
+        <c:axId val="86624128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71680384"/>
+        <c:axId val="86622592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4960,7 +5031,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71681920"/>
+        <c:crossAx val="86624128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4968,7 +5039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71681920"/>
+        <c:axId val="86624128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4979,7 +5050,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71680384"/>
+        <c:crossAx val="86622592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5499,11 +5570,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="71780224"/>
-        <c:axId val="71781760"/>
+        <c:axId val="89999232"/>
+        <c:axId val="90000768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71780224"/>
+        <c:axId val="89999232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5512,7 +5583,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71781760"/>
+        <c:crossAx val="90000768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5520,7 +5591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71781760"/>
+        <c:axId val="90000768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5531,7 +5602,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71780224"/>
+        <c:crossAx val="89999232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5986,11 +6057,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="68737280"/>
-        <c:axId val="69074944"/>
+        <c:axId val="63691008"/>
+        <c:axId val="67440640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68737280"/>
+        <c:axId val="63691008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5999,7 +6070,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69074944"/>
+        <c:crossAx val="67440640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6007,7 +6078,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69074944"/>
+        <c:axId val="67440640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6018,7 +6089,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68737280"/>
+        <c:crossAx val="63691008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6339,7 +6410,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6692,11 +6762,11 @@
         </c:dLbls>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="70714112"/>
-        <c:axId val="70715648"/>
+        <c:axId val="67627648"/>
+        <c:axId val="67649920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70714112"/>
+        <c:axId val="67627648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6705,7 +6775,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70715648"/>
+        <c:crossAx val="67649920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6713,7 +6783,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70715648"/>
+        <c:axId val="67649920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6724,14 +6794,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70714112"/>
+        <c:crossAx val="67627648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6909,7 +6978,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6997,7 +7065,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7361,16 +7428,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>31751</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>186418</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>154215</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>188384</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>249466</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>120348</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8030,12 +8097,12 @@
       <c r="N1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="108" t="s">
+      <c r="O1" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
+      <c r="P1" s="110"/>
+      <c r="Q1" s="110"/>
+      <c r="R1" s="110"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C2" s="61"/>
@@ -8044,12 +8111,12 @@
       <c r="N2" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="107" t="s">
+      <c r="O2" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107"/>
+      <c r="P2" s="109"/>
+      <c r="Q2" s="109"/>
+      <c r="R2" s="109"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -8064,11 +8131,11 @@
       <c r="N3" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="107" t="s">
+      <c r="O3" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="107"/>
-      <c r="Q3" s="107"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -8090,12 +8157,12 @@
       <c r="N4" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="107" t="s">
+      <c r="O4" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="107"/>
-      <c r="Q4" s="107"/>
-      <c r="R4" s="107"/>
+      <c r="P4" s="109"/>
+      <c r="Q4" s="109"/>
+      <c r="R4" s="109"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -8117,12 +8184,12 @@
       <c r="N5" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="107" t="s">
+      <c r="O5" s="109" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="107"/>
-      <c r="Q5" s="107"/>
-      <c r="R5" s="107"/>
+      <c r="P5" s="109"/>
+      <c r="Q5" s="109"/>
+      <c r="R5" s="109"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -8144,12 +8211,12 @@
       <c r="N6" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="107" t="s">
+      <c r="O6" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="107"/>
-      <c r="Q6" s="107"/>
-      <c r="R6" s="107"/>
+      <c r="P6" s="109"/>
+      <c r="Q6" s="109"/>
+      <c r="R6" s="109"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -8164,12 +8231,12 @@
       <c r="N7" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="107" t="s">
+      <c r="O7" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="107"/>
-      <c r="Q7" s="107"/>
-      <c r="R7" s="107"/>
+      <c r="P7" s="109"/>
+      <c r="Q7" s="109"/>
+      <c r="R7" s="109"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -9574,8 +9641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10663,8 +10730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10681,9 +10748,10 @@
     <col min="11" max="11" width="6.85546875" customWidth="1"/>
     <col min="12" max="12" width="8.42578125" customWidth="1"/>
     <col min="14" max="14" width="18.5703125" customWidth="1"/>
-    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="15" max="15" width="25.28515625" customWidth="1"/>
+    <col min="16" max="16" width="29.140625" customWidth="1"/>
     <col min="17" max="17" width="9.140625" customWidth="1"/>
-    <col min="18" max="18" width="8.42578125" customWidth="1"/>
+    <col min="18" max="18" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -11802,7 +11870,7 @@
         <v>25</v>
       </c>
       <c r="U27" s="105">
-        <f t="shared" ref="U27:U29" si="4">SUM(O27:T27)</f>
+        <f t="shared" ref="U27" si="4">SUM(O27:T27)</f>
         <v>51</v>
       </c>
     </row>
@@ -11900,7 +11968,7 @@
         <v>25</v>
       </c>
       <c r="U29" s="105">
-        <f t="shared" ref="U29:U31" si="5">SUM(O29:T29)</f>
+        <f t="shared" ref="U29" si="5">SUM(O29:T29)</f>
         <v>50</v>
       </c>
     </row>
@@ -11952,7 +12020,7 @@
       <c r="L31" s="18"/>
       <c r="N31" s="6"/>
       <c r="O31" s="106">
-        <f t="shared" ref="O31:T31" si="6">SUM(O24:O30)</f>
+        <f t="shared" ref="O31:Q31" si="6">SUM(O24:O30)</f>
         <v>4</v>
       </c>
       <c r="P31" s="106">
@@ -11968,7 +12036,7 @@
         <v>130</v>
       </c>
       <c r="S31" s="106">
-        <f t="shared" ref="S31:U31" si="7">SUM(S24:S30)</f>
+        <f t="shared" ref="S31:T31" si="7">SUM(S24:S30)</f>
         <v>106</v>
       </c>
       <c r="T31" s="106">
@@ -12005,7 +12073,7 @@
       <c r="K33" s="18"/>
       <c r="L33" s="18"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29"/>
       <c r="B34" s="29"/>
       <c r="C34" s="44"/>
@@ -12031,7 +12099,7 @@
       <c r="K35" s="18"/>
       <c r="L35" s="18"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="42"/>
       <c r="D36" s="42"/>
       <c r="E36" s="42"/>
@@ -12070,9 +12138,1222 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z62"/>
+  <sheetViews>
+    <sheetView topLeftCell="G19" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="63" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="63" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="63"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="8" max="14" width="8.7109375" customWidth="1"/>
+    <col min="16" max="16" width="24.7109375" customWidth="1"/>
+    <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="28.42578125" customWidth="1"/>
+    <col min="25" max="25" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="66" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="65">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="65">
+        <v>3</v>
+      </c>
+      <c r="G9" s="118" t="s">
+        <v>318</v>
+      </c>
+      <c r="H9" s="114" t="s">
+        <v>319</v>
+      </c>
+      <c r="I9" s="115"/>
+      <c r="J9" s="115"/>
+      <c r="K9" s="115"/>
+      <c r="L9" s="115"/>
+      <c r="M9" s="115"/>
+      <c r="N9" s="116" t="s">
+        <v>322</v>
+      </c>
+      <c r="P9" s="80" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q9" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="R9" s="89"/>
+      <c r="S9" s="90" t="s">
+        <v>323</v>
+      </c>
+      <c r="U9" s="80" t="s">
+        <v>186</v>
+      </c>
+      <c r="V9" s="88" t="s">
+        <v>292</v>
+      </c>
+      <c r="W9" s="91" t="s">
+        <v>293</v>
+      </c>
+      <c r="X9" s="89" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y9" s="91" t="s">
+        <v>324</v>
+      </c>
+      <c r="Z9" s="90" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="65">
+        <v>3</v>
+      </c>
+      <c r="G10" s="119"/>
+      <c r="H10" s="68" t="s">
+        <v>314</v>
+      </c>
+      <c r="I10" s="68" t="s">
+        <v>315</v>
+      </c>
+      <c r="J10" s="69" t="s">
+        <v>316</v>
+      </c>
+      <c r="K10" s="70" t="s">
+        <v>320</v>
+      </c>
+      <c r="L10" s="69" t="s">
+        <v>317</v>
+      </c>
+      <c r="M10" s="70" t="s">
+        <v>321</v>
+      </c>
+      <c r="N10" s="117"/>
+      <c r="P10" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q10" s="85" t="s">
+        <v>328</v>
+      </c>
+      <c r="R10" s="85">
+        <v>20</v>
+      </c>
+      <c r="S10" s="73">
+        <f>7*20</f>
+        <v>140</v>
+      </c>
+      <c r="U10" s="82" t="s">
+        <v>80</v>
+      </c>
+      <c r="V10" s="84">
+        <v>21</v>
+      </c>
+      <c r="W10" s="85">
+        <v>25</v>
+      </c>
+      <c r="X10" s="73">
+        <v>46</v>
+      </c>
+      <c r="Y10" s="84">
+        <v>500</v>
+      </c>
+      <c r="Z10" s="73">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="65">
+        <v>2</v>
+      </c>
+      <c r="G11" s="71" t="s">
+        <v>281</v>
+      </c>
+      <c r="H11" s="65">
+        <v>0</v>
+      </c>
+      <c r="I11" s="72"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="95"/>
+      <c r="L11" s="72">
+        <v>3</v>
+      </c>
+      <c r="M11" s="72" t="s">
+        <v>342</v>
+      </c>
+      <c r="N11" s="79" t="s">
+        <v>347</v>
+      </c>
+      <c r="P11" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q11" s="73" t="s">
+        <v>327</v>
+      </c>
+      <c r="R11" s="72">
+        <v>30</v>
+      </c>
+      <c r="S11" s="86">
+        <f>9*30</f>
+        <v>270</v>
+      </c>
+      <c r="U11" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="V11" s="78">
+        <v>27</v>
+      </c>
+      <c r="W11" s="72">
+        <v>24</v>
+      </c>
+      <c r="X11" s="78">
+        <v>51</v>
+      </c>
+      <c r="Y11" s="72">
+        <v>720</v>
+      </c>
+      <c r="Z11" s="72">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="G12" s="74" t="s">
+        <v>282</v>
+      </c>
+      <c r="H12" s="65">
+        <v>6</v>
+      </c>
+      <c r="I12" s="72"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="95"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72">
+        <v>29</v>
+      </c>
+      <c r="N12" s="73">
+        <v>35</v>
+      </c>
+      <c r="P12" s="72" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q12" s="73" t="s">
+        <v>329</v>
+      </c>
+      <c r="R12" s="72">
+        <v>25</v>
+      </c>
+      <c r="S12" s="86">
+        <f>17*25</f>
+        <v>425</v>
+      </c>
+      <c r="U12" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="V12" s="78">
+        <v>91</v>
+      </c>
+      <c r="W12" s="72">
+        <v>27</v>
+      </c>
+      <c r="X12" s="78">
+        <v>118</v>
+      </c>
+      <c r="Y12" s="72">
+        <v>675</v>
+      </c>
+      <c r="Z12" s="72">
+        <v>2950</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="65">
+        <v>3</v>
+      </c>
+      <c r="G13" s="74" t="s">
+        <v>283</v>
+      </c>
+      <c r="H13" s="65"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="95"/>
+      <c r="L13" s="72" t="s">
+        <v>338</v>
+      </c>
+      <c r="M13" s="72" t="s">
+        <v>343</v>
+      </c>
+      <c r="N13" s="73">
+        <v>33</v>
+      </c>
+      <c r="P13" s="72" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q13" s="73" t="s">
+        <v>330</v>
+      </c>
+      <c r="R13" s="72">
+        <v>15</v>
+      </c>
+      <c r="S13" s="86">
+        <f>61*15</f>
+        <v>915</v>
+      </c>
+      <c r="U13" s="74" t="s">
+        <v>126</v>
+      </c>
+      <c r="V13" s="78">
+        <v>41</v>
+      </c>
+      <c r="W13" s="72">
+        <v>202</v>
+      </c>
+      <c r="X13" s="78">
+        <v>243</v>
+      </c>
+      <c r="Y13" s="72">
+        <v>3030</v>
+      </c>
+      <c r="Z13" s="72">
+        <v>3645</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="65">
+        <v>3</v>
+      </c>
+      <c r="G14" s="74" t="s">
+        <v>284</v>
+      </c>
+      <c r="H14" s="78"/>
+      <c r="I14" s="72" t="s">
+        <v>336</v>
+      </c>
+      <c r="J14" s="78" t="s">
+        <v>326</v>
+      </c>
+      <c r="K14" s="95"/>
+      <c r="L14" s="72" t="s">
+        <v>339</v>
+      </c>
+      <c r="M14" s="72"/>
+      <c r="N14" s="73" t="s">
+        <v>348</v>
+      </c>
+      <c r="P14" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q14" s="73" t="s">
+        <v>331</v>
+      </c>
+      <c r="R14" s="72">
+        <v>22</v>
+      </c>
+      <c r="S14" s="86">
+        <f>144*22</f>
+        <v>3168</v>
+      </c>
+      <c r="U14" s="74" t="s">
+        <v>187</v>
+      </c>
+      <c r="V14" s="78">
+        <v>0</v>
+      </c>
+      <c r="W14" s="72">
+        <v>293</v>
+      </c>
+      <c r="X14" s="78">
+        <v>293</v>
+      </c>
+      <c r="Y14" s="72">
+        <v>6446</v>
+      </c>
+      <c r="Z14" s="72">
+        <v>6446</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="65">
+        <v>5</v>
+      </c>
+      <c r="G15" s="74" t="s">
+        <v>285</v>
+      </c>
+      <c r="H15" s="65">
+        <v>3</v>
+      </c>
+      <c r="I15" s="72">
+        <v>2</v>
+      </c>
+      <c r="J15" s="78" t="s">
+        <v>337</v>
+      </c>
+      <c r="K15" s="95"/>
+      <c r="L15" s="72" t="s">
+        <v>340</v>
+      </c>
+      <c r="M15" s="72" t="s">
+        <v>344</v>
+      </c>
+      <c r="N15" s="73" t="s">
+        <v>349</v>
+      </c>
+      <c r="P15" s="72" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q15" s="73">
+        <v>0</v>
+      </c>
+      <c r="R15" s="72">
+        <v>15</v>
+      </c>
+      <c r="S15" s="86">
+        <v>0</v>
+      </c>
+      <c r="U15" s="74" t="s">
+        <v>224</v>
+      </c>
+      <c r="V15" s="78">
+        <v>0</v>
+      </c>
+      <c r="W15" s="72">
+        <v>162</v>
+      </c>
+      <c r="X15" s="78">
+        <v>162</v>
+      </c>
+      <c r="Y15" s="72">
+        <v>2430</v>
+      </c>
+      <c r="Z15" s="72">
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="65">
+        <v>2</v>
+      </c>
+      <c r="G16" s="74" t="s">
+        <v>286</v>
+      </c>
+      <c r="H16" s="65" t="s">
+        <v>335</v>
+      </c>
+      <c r="I16" s="72"/>
+      <c r="J16" s="78" t="s">
+        <v>346</v>
+      </c>
+      <c r="K16" s="95"/>
+      <c r="L16" s="72" t="s">
+        <v>341</v>
+      </c>
+      <c r="M16" s="72" t="s">
+        <v>345</v>
+      </c>
+      <c r="N16" s="73" t="s">
+        <v>350</v>
+      </c>
+      <c r="P16" s="103" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q16" s="99">
+        <v>238</v>
+      </c>
+      <c r="R16" s="98"/>
+      <c r="S16" s="99">
+        <f>SUM(S10:S15)</f>
+        <v>4918</v>
+      </c>
+      <c r="U16" s="83" t="s">
+        <v>294</v>
+      </c>
+      <c r="V16" s="92">
+        <v>180</v>
+      </c>
+      <c r="W16" s="87">
+        <v>733</v>
+      </c>
+      <c r="X16" s="92">
+        <v>913</v>
+      </c>
+      <c r="Y16" s="87">
+        <v>13801</v>
+      </c>
+      <c r="Z16" s="87">
+        <v>17921</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="65">
+        <v>3</v>
+      </c>
+      <c r="G17" s="75" t="s">
+        <v>287</v>
+      </c>
+      <c r="H17" s="67"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="77"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="76">
+        <v>5</v>
+      </c>
+      <c r="M17" s="76">
+        <v>30</v>
+      </c>
+      <c r="N17" s="77">
+        <v>35</v>
+      </c>
+      <c r="P17" s="72" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q17" s="100">
+        <v>236</v>
+      </c>
+      <c r="R17" s="97"/>
+      <c r="S17" s="100">
+        <v>4981</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="N18" s="104"/>
+      <c r="P18" s="76" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q18" s="101">
+        <v>-2</v>
+      </c>
+      <c r="R18" s="97"/>
+      <c r="S18" s="102">
+        <f>S16-S17</f>
+        <v>-63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="65">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="94"/>
+      <c r="R21" s="94"/>
+      <c r="S21" s="94"/>
+      <c r="T21" s="94"/>
+      <c r="U21" s="94"/>
+    </row>
+    <row r="22" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="65">
+        <v>3</v>
+      </c>
+      <c r="G22" s="118" t="s">
+        <v>318</v>
+      </c>
+      <c r="H22" s="114" t="s">
+        <v>319</v>
+      </c>
+      <c r="I22" s="115"/>
+      <c r="J22" s="115"/>
+      <c r="K22" s="115"/>
+      <c r="L22" s="115"/>
+      <c r="M22" s="115"/>
+      <c r="N22" s="116" t="s">
+        <v>322</v>
+      </c>
+      <c r="P22" s="108" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q22" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="R22" s="89"/>
+      <c r="S22" s="90" t="s">
+        <v>323</v>
+      </c>
+      <c r="T22" s="93"/>
+      <c r="U22" s="93"/>
+    </row>
+    <row r="23" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="65">
+        <v>2</v>
+      </c>
+      <c r="G23" s="119"/>
+      <c r="H23" s="68" t="s">
+        <v>314</v>
+      </c>
+      <c r="I23" s="68" t="s">
+        <v>315</v>
+      </c>
+      <c r="J23" s="69" t="s">
+        <v>316</v>
+      </c>
+      <c r="K23" s="70" t="s">
+        <v>320</v>
+      </c>
+      <c r="L23" s="69" t="s">
+        <v>317</v>
+      </c>
+      <c r="M23" s="70" t="s">
+        <v>321</v>
+      </c>
+      <c r="N23" s="117"/>
+      <c r="P23" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q23" s="85" t="s">
+        <v>352</v>
+      </c>
+      <c r="R23" s="85">
+        <v>20</v>
+      </c>
+      <c r="S23" s="73">
+        <v>80</v>
+      </c>
+      <c r="T23" s="93"/>
+      <c r="U23" s="93"/>
+    </row>
+    <row r="24" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="65">
+        <v>2</v>
+      </c>
+      <c r="G24" s="71" t="s">
+        <v>281</v>
+      </c>
+      <c r="H24" s="107"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="78"/>
+      <c r="K24" s="121">
+        <v>28</v>
+      </c>
+      <c r="L24" s="72" t="s">
+        <v>358</v>
+      </c>
+      <c r="M24" s="72" t="s">
+        <v>365</v>
+      </c>
+      <c r="N24" s="79">
+        <v>50</v>
+      </c>
+      <c r="P24" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q24" s="73" t="s">
+        <v>353</v>
+      </c>
+      <c r="R24" s="72">
+        <v>30</v>
+      </c>
+      <c r="S24" s="86">
+        <v>120</v>
+      </c>
+      <c r="T24" s="93"/>
+      <c r="U24" s="93"/>
+    </row>
+    <row r="25" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="65">
+        <v>2</v>
+      </c>
+      <c r="G25" s="74" t="s">
+        <v>282</v>
+      </c>
+      <c r="H25" s="107"/>
+      <c r="I25" s="72" t="s">
+        <v>354</v>
+      </c>
+      <c r="J25" s="78"/>
+      <c r="K25" s="121">
+        <v>28</v>
+      </c>
+      <c r="L25" s="72" t="s">
+        <v>359</v>
+      </c>
+      <c r="M25" s="72">
+        <v>12</v>
+      </c>
+      <c r="N25" s="73">
+        <v>51</v>
+      </c>
+      <c r="P25" s="72" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q25" s="73" t="s">
+        <v>354</v>
+      </c>
+      <c r="R25" s="72">
+        <v>25</v>
+      </c>
+      <c r="S25" s="86">
+        <v>50</v>
+      </c>
+      <c r="T25" s="120"/>
+      <c r="U25" s="93"/>
+    </row>
+    <row r="26" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="65">
+        <v>3</v>
+      </c>
+      <c r="G26" s="74" t="s">
+        <v>283</v>
+      </c>
+      <c r="H26" s="107" t="s">
+        <v>353</v>
+      </c>
+      <c r="I26" s="72"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="121">
+        <v>28</v>
+      </c>
+      <c r="L26" s="72" t="s">
+        <v>360</v>
+      </c>
+      <c r="M26" s="72"/>
+      <c r="N26" s="73" t="s">
+        <v>368</v>
+      </c>
+      <c r="P26" s="72" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q26" s="73" t="s">
+        <v>355</v>
+      </c>
+      <c r="R26" s="72">
+        <v>15</v>
+      </c>
+      <c r="S26" s="86">
+        <v>1590</v>
+      </c>
+      <c r="T26" s="93"/>
+      <c r="U26" s="93"/>
+    </row>
+    <row r="27" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="G27" s="74" t="s">
+        <v>284</v>
+      </c>
+      <c r="H27" s="78"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="121" t="s">
+        <v>345</v>
+      </c>
+      <c r="L27" s="72" t="s">
+        <v>361</v>
+      </c>
+      <c r="M27" s="72" t="s">
+        <v>366</v>
+      </c>
+      <c r="N27" s="73" t="s">
+        <v>369</v>
+      </c>
+      <c r="P27" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q27" s="73" t="s">
+        <v>356</v>
+      </c>
+      <c r="R27" s="72">
+        <v>22</v>
+      </c>
+      <c r="S27" s="86">
+        <v>2354</v>
+      </c>
+      <c r="T27" s="93"/>
+      <c r="U27" s="93"/>
+    </row>
+    <row r="28" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="65">
+        <v>6</v>
+      </c>
+      <c r="G28" s="74" t="s">
+        <v>285</v>
+      </c>
+      <c r="H28" s="107"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="78" t="s">
+        <v>354</v>
+      </c>
+      <c r="K28" s="121">
+        <v>10</v>
+      </c>
+      <c r="L28" s="72" t="s">
+        <v>362</v>
+      </c>
+      <c r="M28" s="72" t="s">
+        <v>367</v>
+      </c>
+      <c r="N28" s="73" t="s">
+        <v>370</v>
+      </c>
+      <c r="P28" s="72" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q28" s="73" t="s">
+        <v>357</v>
+      </c>
+      <c r="R28" s="72">
+        <v>15</v>
+      </c>
+      <c r="S28" s="86">
+        <v>1950</v>
+      </c>
+      <c r="T28" s="93"/>
+      <c r="U28" s="93"/>
+    </row>
+    <row r="29" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>309</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>310</v>
+      </c>
+      <c r="G29" s="74" t="s">
+        <v>286</v>
+      </c>
+      <c r="H29" s="107"/>
+      <c r="I29" s="72" t="s">
+        <v>346</v>
+      </c>
+      <c r="J29" s="78"/>
+      <c r="K29" s="121"/>
+      <c r="L29" s="72" t="s">
+        <v>363</v>
+      </c>
+      <c r="M29" s="72" t="s">
+        <v>366</v>
+      </c>
+      <c r="N29" s="73" t="s">
+        <v>368</v>
+      </c>
+      <c r="P29" s="103" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q29" s="99">
+        <v>353</v>
+      </c>
+      <c r="R29" s="98"/>
+      <c r="S29" s="99">
+        <f>SUM(S23:S28)</f>
+        <v>6144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="65">
+        <v>3</v>
+      </c>
+      <c r="G30" s="75" t="s">
+        <v>287</v>
+      </c>
+      <c r="H30" s="67"/>
+      <c r="I30" s="76"/>
+      <c r="J30" s="77"/>
+      <c r="K30" s="67">
+        <v>28</v>
+      </c>
+      <c r="L30" s="76" t="s">
+        <v>364</v>
+      </c>
+      <c r="M30" s="76">
+        <v>18</v>
+      </c>
+      <c r="N30" s="77" t="s">
+        <v>371</v>
+      </c>
+      <c r="P30" s="72" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q30" s="100">
+        <v>345</v>
+      </c>
+      <c r="R30" s="97"/>
+      <c r="S30" s="100">
+        <v>6158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="65">
+        <v>2</v>
+      </c>
+      <c r="P31" s="76" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q31" s="101">
+        <f>Q30-Q29</f>
+        <v>-8</v>
+      </c>
+      <c r="R31" s="97"/>
+      <c r="S31" s="102">
+        <f>S30-S29</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32"/>
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33"/>
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="65" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="64"/>
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="N22:N23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="O3" sqref="O3:Q9"/>
     </sheetView>
   </sheetViews>
@@ -13085,12 +14366,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG28" sqref="AG28:AM34"/>
+    <sheetView topLeftCell="T1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AK3" sqref="AK3:AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13110,59 +14391,62 @@
     <col min="22" max="22" width="11.42578125" customWidth="1"/>
     <col min="23" max="23" width="20.28515625" customWidth="1"/>
     <col min="28" max="28" width="20.42578125" customWidth="1"/>
+    <col min="36" max="36" width="14.42578125" customWidth="1"/>
+    <col min="37" max="37" width="18.140625" customWidth="1"/>
+    <col min="40" max="40" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="113" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="J1" s="109" t="s">
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="J1" s="111" t="s">
         <v>289</v>
       </c>
-      <c r="K1" s="109"/>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="109"/>
-      <c r="P1" s="109"/>
-      <c r="Q1" s="109"/>
-      <c r="S1" s="109" t="s">
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
+      <c r="S1" s="111" t="s">
         <v>290</v>
       </c>
-      <c r="T1" s="109"/>
-      <c r="U1" s="109"/>
-      <c r="V1" s="109"/>
-      <c r="W1" s="109"/>
-      <c r="X1" s="109"/>
-      <c r="Y1" s="109"/>
-      <c r="Z1" s="109"/>
-      <c r="AB1" s="109" t="s">
+      <c r="T1" s="111"/>
+      <c r="U1" s="111"/>
+      <c r="V1" s="111"/>
+      <c r="W1" s="111"/>
+      <c r="X1" s="111"/>
+      <c r="Y1" s="111"/>
+      <c r="Z1" s="111"/>
+      <c r="AB1" s="111" t="s">
         <v>219</v>
       </c>
-      <c r="AC1" s="109"/>
-      <c r="AD1" s="109"/>
-      <c r="AE1" s="109"/>
-      <c r="AF1" s="109"/>
-      <c r="AG1" s="109"/>
-      <c r="AH1" s="109"/>
-      <c r="AI1" s="109"/>
-      <c r="AK1" s="109" t="s">
+      <c r="AC1" s="111"/>
+      <c r="AD1" s="111"/>
+      <c r="AE1" s="111"/>
+      <c r="AF1" s="111"/>
+      <c r="AG1" s="111"/>
+      <c r="AH1" s="111"/>
+      <c r="AI1" s="111"/>
+      <c r="AK1" s="111" t="s">
         <v>291</v>
       </c>
-      <c r="AL1" s="109"/>
-      <c r="AM1" s="109"/>
-      <c r="AN1" s="109"/>
-      <c r="AO1" s="109"/>
-      <c r="AP1" s="109"/>
-      <c r="AQ1" s="109"/>
-      <c r="AR1" s="109"/>
+      <c r="AL1" s="111"/>
+      <c r="AM1" s="111"/>
+      <c r="AN1" s="111"/>
+      <c r="AO1" s="111"/>
+      <c r="AP1" s="111"/>
+      <c r="AQ1" s="111"/>
+      <c r="AR1" s="111"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
@@ -14677,26 +15961,26 @@
       </c>
     </row>
     <row r="27" spans="1:44" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H27" s="110" t="s">
+      <c r="H27" s="112" t="s">
         <v>307</v>
       </c>
-      <c r="I27" s="110"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="110"/>
-      <c r="L27" s="110"/>
-      <c r="M27" s="110"/>
-      <c r="N27" s="110"/>
-      <c r="O27" s="110"/>
-      <c r="W27" s="110" t="s">
+      <c r="I27" s="112"/>
+      <c r="J27" s="112"/>
+      <c r="K27" s="112"/>
+      <c r="L27" s="112"/>
+      <c r="M27" s="112"/>
+      <c r="N27" s="112"/>
+      <c r="O27" s="112"/>
+      <c r="W27" s="112" t="s">
         <v>308</v>
       </c>
-      <c r="X27" s="109"/>
-      <c r="Y27" s="109"/>
-      <c r="Z27" s="109"/>
-      <c r="AA27" s="109"/>
-      <c r="AB27" s="109"/>
-      <c r="AC27" s="109"/>
-      <c r="AD27" s="109"/>
+      <c r="X27" s="111"/>
+      <c r="Y27" s="111"/>
+      <c r="Z27" s="111"/>
+      <c r="AA27" s="111"/>
+      <c r="AB27" s="111"/>
+      <c r="AC27" s="111"/>
+      <c r="AD27" s="111"/>
     </row>
     <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -15603,956 +16887,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z62"/>
-  <sheetViews>
-    <sheetView topLeftCell="G4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="63" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="63" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="63"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="14" width="8.7109375" customWidth="1"/>
-    <col min="16" max="16" width="24.7109375" customWidth="1"/>
-    <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="28.42578125" customWidth="1"/>
-    <col min="25" max="25" width="23.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
-        <v>311</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="66" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="65">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="65">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="65" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="65" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="65">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="65" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="65">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="65" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="65">
-        <v>3</v>
-      </c>
-      <c r="G9" s="116" t="s">
-        <v>318</v>
-      </c>
-      <c r="H9" s="112" t="s">
-        <v>319</v>
-      </c>
-      <c r="I9" s="113"/>
-      <c r="J9" s="113"/>
-      <c r="K9" s="113"/>
-      <c r="L9" s="113"/>
-      <c r="M9" s="113"/>
-      <c r="N9" s="114" t="s">
-        <v>322</v>
-      </c>
-      <c r="P9" s="80" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q9" s="91" t="s">
-        <v>3</v>
-      </c>
-      <c r="R9" s="89"/>
-      <c r="S9" s="90" t="s">
-        <v>323</v>
-      </c>
-      <c r="U9" s="80" t="s">
-        <v>186</v>
-      </c>
-      <c r="V9" s="88" t="s">
-        <v>292</v>
-      </c>
-      <c r="W9" s="91" t="s">
-        <v>293</v>
-      </c>
-      <c r="X9" s="89" t="s">
-        <v>294</v>
-      </c>
-      <c r="Y9" s="91" t="s">
-        <v>324</v>
-      </c>
-      <c r="Z9" s="90" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="65" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" s="65">
-        <v>3</v>
-      </c>
-      <c r="G10" s="117"/>
-      <c r="H10" s="68" t="s">
-        <v>314</v>
-      </c>
-      <c r="I10" s="68" t="s">
-        <v>315</v>
-      </c>
-      <c r="J10" s="69" t="s">
-        <v>316</v>
-      </c>
-      <c r="K10" s="70" t="s">
-        <v>320</v>
-      </c>
-      <c r="L10" s="69" t="s">
-        <v>317</v>
-      </c>
-      <c r="M10" s="70" t="s">
-        <v>321</v>
-      </c>
-      <c r="N10" s="115"/>
-      <c r="P10" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q10" s="85" t="s">
-        <v>328</v>
-      </c>
-      <c r="R10" s="85">
-        <v>20</v>
-      </c>
-      <c r="S10" s="73">
-        <f>7*20</f>
-        <v>140</v>
-      </c>
-      <c r="U10" s="82" t="s">
-        <v>80</v>
-      </c>
-      <c r="V10" s="84">
-        <v>21</v>
-      </c>
-      <c r="W10" s="85">
-        <v>25</v>
-      </c>
-      <c r="X10" s="73">
-        <v>46</v>
-      </c>
-      <c r="Y10" s="84">
-        <v>500</v>
-      </c>
-      <c r="Z10" s="73">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="65" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="65">
-        <v>2</v>
-      </c>
-      <c r="G11" s="71" t="s">
-        <v>281</v>
-      </c>
-      <c r="H11" s="65">
-        <v>0</v>
-      </c>
-      <c r="I11" s="72"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="95"/>
-      <c r="L11" s="72">
-        <v>3</v>
-      </c>
-      <c r="M11" s="72" t="s">
-        <v>342</v>
-      </c>
-      <c r="N11" s="79" t="s">
-        <v>347</v>
-      </c>
-      <c r="P11" s="72" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q11" s="73" t="s">
-        <v>327</v>
-      </c>
-      <c r="R11" s="72">
-        <v>30</v>
-      </c>
-      <c r="S11" s="86">
-        <f>9*30</f>
-        <v>270</v>
-      </c>
-      <c r="U11" s="74" t="s">
-        <v>90</v>
-      </c>
-      <c r="V11" s="78">
-        <v>27</v>
-      </c>
-      <c r="W11" s="72">
-        <v>24</v>
-      </c>
-      <c r="X11" s="78">
-        <v>51</v>
-      </c>
-      <c r="Y11" s="72">
-        <v>720</v>
-      </c>
-      <c r="Z11" s="72">
-        <v>1530</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="G12" s="74" t="s">
-        <v>282</v>
-      </c>
-      <c r="H12" s="65">
-        <v>6</v>
-      </c>
-      <c r="I12" s="72"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="95"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72">
-        <v>29</v>
-      </c>
-      <c r="N12" s="73">
-        <v>35</v>
-      </c>
-      <c r="P12" s="72" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q12" s="73" t="s">
-        <v>329</v>
-      </c>
-      <c r="R12" s="72">
-        <v>25</v>
-      </c>
-      <c r="S12" s="86">
-        <f>17*25</f>
-        <v>425</v>
-      </c>
-      <c r="U12" s="74" t="s">
-        <v>188</v>
-      </c>
-      <c r="V12" s="78">
-        <v>91</v>
-      </c>
-      <c r="W12" s="72">
-        <v>27</v>
-      </c>
-      <c r="X12" s="78">
-        <v>118</v>
-      </c>
-      <c r="Y12" s="72">
-        <v>675</v>
-      </c>
-      <c r="Z12" s="72">
-        <v>2950</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="65" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="65">
-        <v>3</v>
-      </c>
-      <c r="G13" s="74" t="s">
-        <v>283</v>
-      </c>
-      <c r="H13" s="65"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="95"/>
-      <c r="L13" s="72" t="s">
-        <v>338</v>
-      </c>
-      <c r="M13" s="72" t="s">
-        <v>343</v>
-      </c>
-      <c r="N13" s="73">
-        <v>33</v>
-      </c>
-      <c r="P13" s="72" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q13" s="73" t="s">
-        <v>330</v>
-      </c>
-      <c r="R13" s="72">
-        <v>15</v>
-      </c>
-      <c r="S13" s="86">
-        <f>61*15</f>
-        <v>915</v>
-      </c>
-      <c r="U13" s="74" t="s">
-        <v>126</v>
-      </c>
-      <c r="V13" s="78">
-        <v>41</v>
-      </c>
-      <c r="W13" s="72">
-        <v>202</v>
-      </c>
-      <c r="X13" s="78">
-        <v>243</v>
-      </c>
-      <c r="Y13" s="72">
-        <v>3030</v>
-      </c>
-      <c r="Z13" s="72">
-        <v>3645</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="65" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="65">
-        <v>3</v>
-      </c>
-      <c r="G14" s="74" t="s">
-        <v>284</v>
-      </c>
-      <c r="H14" s="78"/>
-      <c r="I14" s="72" t="s">
-        <v>336</v>
-      </c>
-      <c r="J14" s="78" t="s">
-        <v>326</v>
-      </c>
-      <c r="K14" s="95"/>
-      <c r="L14" s="72" t="s">
-        <v>339</v>
-      </c>
-      <c r="M14" s="72"/>
-      <c r="N14" s="73" t="s">
-        <v>348</v>
-      </c>
-      <c r="P14" s="72" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q14" s="73" t="s">
-        <v>331</v>
-      </c>
-      <c r="R14" s="72">
-        <v>22</v>
-      </c>
-      <c r="S14" s="86">
-        <f>144*22</f>
-        <v>3168</v>
-      </c>
-      <c r="U14" s="74" t="s">
-        <v>187</v>
-      </c>
-      <c r="V14" s="78">
-        <v>0</v>
-      </c>
-      <c r="W14" s="72">
-        <v>293</v>
-      </c>
-      <c r="X14" s="78">
-        <v>293</v>
-      </c>
-      <c r="Y14" s="72">
-        <v>6446</v>
-      </c>
-      <c r="Z14" s="72">
-        <v>6446</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="65">
-        <v>5</v>
-      </c>
-      <c r="G15" s="74" t="s">
-        <v>285</v>
-      </c>
-      <c r="H15" s="65">
-        <v>3</v>
-      </c>
-      <c r="I15" s="72">
-        <v>2</v>
-      </c>
-      <c r="J15" s="78" t="s">
-        <v>337</v>
-      </c>
-      <c r="K15" s="95"/>
-      <c r="L15" s="72" t="s">
-        <v>340</v>
-      </c>
-      <c r="M15" s="72" t="s">
-        <v>344</v>
-      </c>
-      <c r="N15" s="73" t="s">
-        <v>349</v>
-      </c>
-      <c r="P15" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q15" s="73">
-        <v>0</v>
-      </c>
-      <c r="R15" s="72">
-        <v>15</v>
-      </c>
-      <c r="S15" s="86">
-        <v>0</v>
-      </c>
-      <c r="U15" s="74" t="s">
-        <v>224</v>
-      </c>
-      <c r="V15" s="78">
-        <v>0</v>
-      </c>
-      <c r="W15" s="72">
-        <v>162</v>
-      </c>
-      <c r="X15" s="78">
-        <v>162</v>
-      </c>
-      <c r="Y15" s="72">
-        <v>2430</v>
-      </c>
-      <c r="Z15" s="72">
-        <v>2430</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="65">
-        <v>2</v>
-      </c>
-      <c r="G16" s="74" t="s">
-        <v>286</v>
-      </c>
-      <c r="H16" s="65" t="s">
-        <v>335</v>
-      </c>
-      <c r="I16" s="72"/>
-      <c r="J16" s="78" t="s">
-        <v>346</v>
-      </c>
-      <c r="K16" s="95"/>
-      <c r="L16" s="72" t="s">
-        <v>341</v>
-      </c>
-      <c r="M16" s="72" t="s">
-        <v>345</v>
-      </c>
-      <c r="N16" s="73" t="s">
-        <v>350</v>
-      </c>
-      <c r="P16" s="103" t="s">
-        <v>332</v>
-      </c>
-      <c r="Q16" s="99">
-        <v>238</v>
-      </c>
-      <c r="R16" s="98"/>
-      <c r="S16" s="99">
-        <f>SUM(S10:S15)</f>
-        <v>4918</v>
-      </c>
-      <c r="U16" s="83" t="s">
-        <v>294</v>
-      </c>
-      <c r="V16" s="92">
-        <v>180</v>
-      </c>
-      <c r="W16" s="87">
-        <v>733</v>
-      </c>
-      <c r="X16" s="92">
-        <v>913</v>
-      </c>
-      <c r="Y16" s="87">
-        <v>13801</v>
-      </c>
-      <c r="Z16" s="87">
-        <v>17921</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="21" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="D17" s="65">
-        <v>3</v>
-      </c>
-      <c r="G17" s="75" t="s">
-        <v>287</v>
-      </c>
-      <c r="H17" s="67"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="77"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="76">
-        <v>5</v>
-      </c>
-      <c r="M17" s="76">
-        <v>30</v>
-      </c>
-      <c r="N17" s="77">
-        <v>35</v>
-      </c>
-      <c r="P17" s="72" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q17" s="100">
-        <v>236</v>
-      </c>
-      <c r="R17" s="97"/>
-      <c r="S17" s="100">
-        <v>4981</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="21" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="N18" s="104"/>
-      <c r="P18" s="76" t="s">
-        <v>334</v>
-      </c>
-      <c r="Q18" s="101">
-        <v>-2</v>
-      </c>
-      <c r="R18" s="97"/>
-      <c r="S18" s="102">
-        <f>S16-S17</f>
-        <v>-63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="65">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="65">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="65">
-        <v>4</v>
-      </c>
-      <c r="Q21" s="94"/>
-      <c r="R21" s="94"/>
-      <c r="S21" s="94"/>
-      <c r="T21" s="94"/>
-      <c r="U21" s="94"/>
-    </row>
-    <row r="22" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="65">
-        <v>3</v>
-      </c>
-      <c r="Q22" s="93"/>
-      <c r="R22" s="93"/>
-      <c r="S22" s="93"/>
-      <c r="T22" s="93"/>
-      <c r="U22" s="93"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="65">
-        <v>2</v>
-      </c>
-      <c r="Q23" s="93"/>
-      <c r="R23" s="93"/>
-      <c r="S23" s="93"/>
-      <c r="T23" s="93"/>
-      <c r="U23" s="93"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="65">
-        <v>2</v>
-      </c>
-      <c r="Q24" s="93"/>
-      <c r="R24" s="93"/>
-      <c r="S24" s="93"/>
-      <c r="T24" s="93"/>
-      <c r="U24" s="93"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="65" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="65">
-        <v>2</v>
-      </c>
-      <c r="Q25" s="93"/>
-      <c r="R25" s="93"/>
-      <c r="S25" s="93"/>
-      <c r="T25" s="93"/>
-      <c r="U25" s="93"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="65">
-        <v>3</v>
-      </c>
-      <c r="Q26" s="93"/>
-      <c r="R26" s="93"/>
-      <c r="S26" s="93"/>
-      <c r="T26" s="93"/>
-      <c r="U26" s="93"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="Q27" s="93"/>
-      <c r="R27" s="93"/>
-      <c r="S27" s="93"/>
-      <c r="T27" s="93"/>
-      <c r="U27" s="93"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="65">
-        <v>6</v>
-      </c>
-      <c r="Q28" s="93"/>
-      <c r="R28" s="93"/>
-      <c r="S28" s="93"/>
-      <c r="T28" s="93"/>
-      <c r="U28" s="93"/>
-    </row>
-    <row r="29" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="32" t="s">
-        <v>309</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>70</v>
-      </c>
-      <c r="B30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="65" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="65">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32"/>
-      <c r="D32"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33"/>
-      <c r="D33"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="65" t="s">
-        <v>91</v>
-      </c>
-      <c r="D34" s="65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="64"/>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="G9:G10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>